<commit_message>
fix: balance scorecard minimum value threshold
</commit_message>
<xml_diff>
--- a/templates/management/Balance Scorecard (BSC).xlsx
+++ b/templates/management/Balance Scorecard (BSC).xlsx
@@ -413,8 +413,8 @@
       <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
       <border/>
@@ -423,8 +423,8 @@
       <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
       <border/>
@@ -663,6 +663,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <tabColor rgb="FF9900FF"/>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
@@ -688,211 +689,211 @@
       <c r="E1" s="3"/>
       <c r="F1" s="4">
         <f t="shared" ref="F1:BE1" si="1">AVERAGEIFS(F9:F1013,$E9:$E1013,"% Target")</f>
-        <v>0.4201954451</v>
+        <v>0.4452685879</v>
       </c>
       <c r="G1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4443596264</v>
+        <v>0.4422457692</v>
       </c>
       <c r="H1" s="4">
         <f t="shared" si="1"/>
-        <v>0.3648119286</v>
+        <v>0.3023463571</v>
       </c>
       <c r="I1" s="4">
         <f t="shared" si="1"/>
-        <v>0.569029989</v>
+        <v>0.5258767033</v>
       </c>
       <c r="J1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5740620275</v>
+        <v>0.643591456</v>
       </c>
       <c r="K1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4436682088</v>
+        <v>0.4728619231</v>
       </c>
       <c r="L1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4879322473</v>
+        <v>0.521355533</v>
       </c>
       <c r="M1" s="4">
         <f t="shared" si="1"/>
-        <v>0.539232</v>
+        <v>0.5647217143</v>
       </c>
       <c r="N1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4853046099</v>
+        <v>0.5485270385</v>
       </c>
       <c r="O1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5330096484</v>
+        <v>0.5968060769</v>
       </c>
       <c r="P1" s="4">
         <f t="shared" si="1"/>
-        <v>0.567304544</v>
+        <v>0.519619544</v>
       </c>
       <c r="Q1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5308415824</v>
+        <v>0.4830432967</v>
       </c>
       <c r="R1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4769997637</v>
+        <v>0.4530146209</v>
       </c>
       <c r="S1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6080312308</v>
+        <v>0.4581923736</v>
       </c>
       <c r="T1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5427012692</v>
+        <v>0.5480889835</v>
       </c>
       <c r="U1" s="4">
         <f t="shared" si="1"/>
-        <v>0.656211022</v>
+        <v>0.5566083077</v>
       </c>
       <c r="V1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6759320604</v>
+        <v>0.6282593462</v>
       </c>
       <c r="W1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6583080989</v>
+        <v>0.5705382418</v>
       </c>
       <c r="X1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6139065659</v>
+        <v>0.6166417088</v>
       </c>
       <c r="Y1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5754547473</v>
+        <v>0.6716047473</v>
       </c>
       <c r="Z1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6700359286</v>
+        <v>0.6892907857</v>
       </c>
       <c r="AA1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7526726813</v>
+        <v>0.6739615385</v>
       </c>
       <c r="AB1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7969724341</v>
+        <v>0.7963160055</v>
       </c>
       <c r="AC1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6992796154</v>
+        <v>0.6544556154</v>
       </c>
       <c r="AD1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6736079396</v>
+        <v>0.7866706538</v>
       </c>
       <c r="AE1" s="4">
         <f t="shared" si="1"/>
-        <v>0.716287978</v>
+        <v>0.7877746923</v>
       </c>
       <c r="AF1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6926508736</v>
+        <v>0.6972191593</v>
       </c>
       <c r="AG1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7809494835</v>
+        <v>0.7612441978</v>
       </c>
       <c r="AH1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7869022363</v>
+        <v>0.8846829505</v>
       </c>
       <c r="AI1" s="4">
         <f t="shared" si="1"/>
-        <v>0.853170989</v>
+        <v>0.8387987033</v>
       </c>
       <c r="AJ1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7099380275</v>
+        <v>0.806668456</v>
       </c>
       <c r="AK1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7372789231</v>
+        <v>0.7493352088</v>
       </c>
       <c r="AL1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8966981044</v>
+        <v>0.8758983901</v>
       </c>
       <c r="AM1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9056475714</v>
+        <v>0.8759904286</v>
       </c>
       <c r="AN1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8745450385</v>
+        <v>0.8141698956</v>
       </c>
       <c r="AO1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8999780769</v>
+        <v>0.8164377912</v>
       </c>
       <c r="AP1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7991861154</v>
+        <v>0.8841892582</v>
       </c>
       <c r="AQ1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9137921538</v>
+        <v>0.8923211538</v>
       </c>
       <c r="AR1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9112330495</v>
+        <v>0.8003207637</v>
       </c>
       <c r="AS1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9237236593</v>
+        <v>0.9983748022</v>
       </c>
       <c r="AT1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9959638407</v>
+        <v>0.9738076978</v>
       </c>
       <c r="AU1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8785238791</v>
+        <v>0.8872597363</v>
       </c>
       <c r="AV1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9648100604</v>
+        <v>0.9456257747</v>
       </c>
       <c r="AW1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9524203846</v>
+        <v>0.9609923846</v>
       </c>
       <c r="AX1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9558717088</v>
+        <v>0.9905724231</v>
       </c>
       <c r="AY1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9191433187</v>
+        <v>1.03586789</v>
       </c>
       <c r="AZ1" s="4">
         <f t="shared" si="1"/>
-        <v>1.176788643</v>
+        <v>1.093406214</v>
       </c>
       <c r="BA1" s="4">
         <f t="shared" si="1"/>
-        <v>1.01241011</v>
+        <v>0.9525403956</v>
       </c>
       <c r="BB1" s="4">
         <f t="shared" si="1"/>
-        <v>1.006098863</v>
+        <v>0.9689434341</v>
       </c>
       <c r="BC1" s="4">
         <f t="shared" si="1"/>
-        <v>1.049173758</v>
+        <v>1.081434187</v>
       </c>
       <c r="BD1" s="4">
         <f t="shared" si="1"/>
-        <v>1.112331654</v>
+        <v>1.00382794</v>
       </c>
       <c r="BE1" s="4">
         <f t="shared" si="1"/>
-        <v>1.152550407</v>
+        <v>1.069283407</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -1348,7 +1349,7 @@
       <c r="B9" s="19"/>
       <c r="C9" s="20">
         <f>SUMIFS(C10:C1013,A10:A1013,A10)</f>
-        <v>0.904098967</v>
+        <v>0.885016633</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="22"/>
@@ -1414,7 +1415,7 @@
       </c>
       <c r="C10" s="25">
         <f t="array" ref="C10">IF( B11="Short-Term", AVERAGE(F12:BE12)*B12, INDEX(F12:BE12, 1, COUNTA(F12:BE12))*B12 )</f>
-        <v>0.3058352308</v>
+        <v>0.3030303692</v>
       </c>
       <c r="D10" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B11=""Short-Term"", SPARKLINE(F12:BE12,IF(B10=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F12:BE12, 1, COUNTA(F12:BE12)) ,IF(B10=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -1425,211 +1426,211 @@
       </c>
       <c r="F10" s="26">
         <f t="shared" ref="F10:BE10" si="2">RANDBETWEEN(100000,150000)</f>
-        <v>149078</v>
+        <v>127419</v>
       </c>
       <c r="G10" s="26">
         <f t="shared" si="2"/>
-        <v>108111</v>
+        <v>104640</v>
       </c>
       <c r="H10" s="26">
         <f t="shared" si="2"/>
-        <v>139053</v>
+        <v>113891</v>
       </c>
       <c r="I10" s="26">
         <f t="shared" si="2"/>
-        <v>137894</v>
+        <v>133580</v>
       </c>
       <c r="J10" s="26">
         <f t="shared" si="2"/>
-        <v>141402</v>
+        <v>149485</v>
       </c>
       <c r="K10" s="26">
         <f t="shared" si="2"/>
-        <v>100127</v>
+        <v>149285</v>
       </c>
       <c r="L10" s="26">
         <f t="shared" si="2"/>
-        <v>131867</v>
+        <v>115951</v>
       </c>
       <c r="M10" s="26">
         <f t="shared" si="2"/>
-        <v>146607</v>
+        <v>136436</v>
       </c>
       <c r="N10" s="26">
         <f t="shared" si="2"/>
-        <v>125102</v>
+        <v>129128</v>
       </c>
       <c r="O10" s="26">
         <f t="shared" si="2"/>
-        <v>119783</v>
+        <v>116758</v>
       </c>
       <c r="P10" s="26">
         <f t="shared" si="2"/>
-        <v>146036</v>
+        <v>116476</v>
       </c>
       <c r="Q10" s="26">
         <f t="shared" si="2"/>
-        <v>100799</v>
+        <v>102465</v>
       </c>
       <c r="R10" s="26">
         <f t="shared" si="2"/>
-        <v>133326</v>
+        <v>125698</v>
       </c>
       <c r="S10" s="26">
         <f t="shared" si="2"/>
-        <v>142512</v>
+        <v>111066</v>
       </c>
       <c r="T10" s="26">
         <f t="shared" si="2"/>
-        <v>102283</v>
+        <v>145260</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="2"/>
-        <v>120983</v>
+        <v>125291</v>
       </c>
       <c r="V10" s="26">
         <f t="shared" si="2"/>
-        <v>132930</v>
+        <v>108293</v>
       </c>
       <c r="W10" s="26">
         <f t="shared" si="2"/>
-        <v>143157</v>
+        <v>106155</v>
       </c>
       <c r="X10" s="26">
         <f t="shared" si="2"/>
-        <v>129785</v>
+        <v>120913</v>
       </c>
       <c r="Y10" s="26">
         <f t="shared" si="2"/>
-        <v>116452</v>
+        <v>134727</v>
       </c>
       <c r="Z10" s="26">
         <f t="shared" si="2"/>
-        <v>134777</v>
+        <v>141139</v>
       </c>
       <c r="AA10" s="26">
         <f t="shared" si="2"/>
-        <v>137354</v>
+        <v>104625</v>
       </c>
       <c r="AB10" s="26">
         <f t="shared" si="2"/>
-        <v>144344</v>
+        <v>148134</v>
       </c>
       <c r="AC10" s="26">
         <f t="shared" si="2"/>
-        <v>111145</v>
+        <v>105196</v>
       </c>
       <c r="AD10" s="26">
         <f t="shared" si="2"/>
-        <v>149235</v>
+        <v>133887</v>
       </c>
       <c r="AE10" s="26">
         <f t="shared" si="2"/>
-        <v>107391</v>
+        <v>136967</v>
       </c>
       <c r="AF10" s="26">
         <f t="shared" si="2"/>
-        <v>138212</v>
+        <v>122691</v>
       </c>
       <c r="AG10" s="26">
         <f t="shared" si="2"/>
-        <v>144933</v>
+        <v>130442</v>
       </c>
       <c r="AH10" s="26">
         <f t="shared" si="2"/>
-        <v>149326</v>
+        <v>142446</v>
       </c>
       <c r="AI10" s="26">
         <f t="shared" si="2"/>
-        <v>133910</v>
+        <v>135377</v>
       </c>
       <c r="AJ10" s="26">
         <f t="shared" si="2"/>
-        <v>148653</v>
+        <v>126812</v>
       </c>
       <c r="AK10" s="26">
         <f t="shared" si="2"/>
-        <v>128952</v>
+        <v>106044</v>
       </c>
       <c r="AL10" s="26">
         <f t="shared" si="2"/>
-        <v>132490</v>
+        <v>147351</v>
       </c>
       <c r="AM10" s="26">
         <f t="shared" si="2"/>
-        <v>129094</v>
+        <v>144044</v>
       </c>
       <c r="AN10" s="26">
         <f t="shared" si="2"/>
-        <v>145521</v>
+        <v>139878</v>
       </c>
       <c r="AO10" s="26">
         <f t="shared" si="2"/>
-        <v>133680</v>
+        <v>121104</v>
       </c>
       <c r="AP10" s="26">
         <f t="shared" si="2"/>
-        <v>102114</v>
+        <v>142260</v>
       </c>
       <c r="AQ10" s="26">
         <f t="shared" si="2"/>
-        <v>105321</v>
+        <v>132100</v>
       </c>
       <c r="AR10" s="26">
         <f t="shared" si="2"/>
-        <v>127720</v>
+        <v>120647</v>
       </c>
       <c r="AS10" s="26">
         <f t="shared" si="2"/>
-        <v>127508</v>
+        <v>121802</v>
       </c>
       <c r="AT10" s="26">
         <f t="shared" si="2"/>
-        <v>121617</v>
+        <v>134693</v>
       </c>
       <c r="AU10" s="26">
         <f t="shared" si="2"/>
-        <v>115653</v>
+        <v>106371</v>
       </c>
       <c r="AV10" s="26">
         <f t="shared" si="2"/>
-        <v>144683</v>
+        <v>137588</v>
       </c>
       <c r="AW10" s="26">
         <f t="shared" si="2"/>
-        <v>111805</v>
+        <v>122502</v>
       </c>
       <c r="AX10" s="26">
         <f t="shared" si="2"/>
-        <v>127143</v>
+        <v>144808</v>
       </c>
       <c r="AY10" s="26">
         <f t="shared" si="2"/>
-        <v>118962</v>
+        <v>128508</v>
       </c>
       <c r="AZ10" s="26">
         <f t="shared" si="2"/>
-        <v>111744</v>
+        <v>133308</v>
       </c>
       <c r="BA10" s="26">
         <f t="shared" si="2"/>
-        <v>115645</v>
+        <v>104561</v>
       </c>
       <c r="BB10" s="26">
         <f t="shared" si="2"/>
-        <v>119774</v>
+        <v>135690</v>
       </c>
       <c r="BC10" s="26">
         <f t="shared" si="2"/>
-        <v>103057</v>
+        <v>125121</v>
       </c>
       <c r="BD10" s="26">
         <f t="shared" si="2"/>
-        <v>117673</v>
+        <v>107580</v>
       </c>
       <c r="BE10" s="26">
         <f t="shared" si="2"/>
-        <v>119707</v>
+        <v>109065</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -1808,211 +1809,211 @@
       </c>
       <c r="F12" s="29">
         <f t="shared" ref="F12:BE12" si="3">IF( $B10="Maximum", F10/F11 , IF( 100%-(F10-F11)/F11 &gt; 0, 100%-(F10-F11)/F11, 0) )</f>
-        <v>1.192624</v>
+        <v>1.019352</v>
       </c>
       <c r="G12" s="29">
         <f t="shared" si="3"/>
-        <v>0.864888</v>
+        <v>0.83712</v>
       </c>
       <c r="H12" s="29">
         <f t="shared" si="3"/>
-        <v>1.112424</v>
+        <v>0.911128</v>
       </c>
       <c r="I12" s="29">
         <f t="shared" si="3"/>
-        <v>1.103152</v>
+        <v>1.06864</v>
       </c>
       <c r="J12" s="29">
         <f t="shared" si="3"/>
-        <v>1.131216</v>
+        <v>1.19588</v>
       </c>
       <c r="K12" s="29">
         <f t="shared" si="3"/>
-        <v>0.801016</v>
+        <v>1.19428</v>
       </c>
       <c r="L12" s="29">
         <f t="shared" si="3"/>
-        <v>1.054936</v>
+        <v>0.927608</v>
       </c>
       <c r="M12" s="29">
         <f t="shared" si="3"/>
-        <v>1.172856</v>
+        <v>1.091488</v>
       </c>
       <c r="N12" s="29">
         <f t="shared" si="3"/>
-        <v>1.000816</v>
+        <v>1.033024</v>
       </c>
       <c r="O12" s="29">
         <f t="shared" si="3"/>
-        <v>0.958264</v>
+        <v>0.934064</v>
       </c>
       <c r="P12" s="29">
         <f t="shared" si="3"/>
-        <v>1.168288</v>
+        <v>0.931808</v>
       </c>
       <c r="Q12" s="29">
         <f t="shared" si="3"/>
-        <v>0.806392</v>
+        <v>0.81972</v>
       </c>
       <c r="R12" s="29">
         <f t="shared" si="3"/>
-        <v>1.066608</v>
+        <v>1.005584</v>
       </c>
       <c r="S12" s="29">
         <f t="shared" si="3"/>
-        <v>1.140096</v>
+        <v>0.888528</v>
       </c>
       <c r="T12" s="29">
         <f t="shared" si="3"/>
-        <v>0.818264</v>
+        <v>1.16208</v>
       </c>
       <c r="U12" s="29">
         <f t="shared" si="3"/>
-        <v>0.967864</v>
+        <v>1.002328</v>
       </c>
       <c r="V12" s="29">
         <f t="shared" si="3"/>
-        <v>1.06344</v>
+        <v>0.866344</v>
       </c>
       <c r="W12" s="29">
         <f t="shared" si="3"/>
-        <v>1.145256</v>
+        <v>0.84924</v>
       </c>
       <c r="X12" s="29">
         <f t="shared" si="3"/>
-        <v>1.03828</v>
+        <v>0.967304</v>
       </c>
       <c r="Y12" s="29">
         <f t="shared" si="3"/>
-        <v>0.931616</v>
+        <v>1.077816</v>
       </c>
       <c r="Z12" s="29">
         <f t="shared" si="3"/>
-        <v>1.078216</v>
+        <v>1.129112</v>
       </c>
       <c r="AA12" s="29">
         <f t="shared" si="3"/>
-        <v>1.098832</v>
+        <v>0.837</v>
       </c>
       <c r="AB12" s="29">
         <f t="shared" si="3"/>
-        <v>1.154752</v>
+        <v>1.185072</v>
       </c>
       <c r="AC12" s="29">
         <f t="shared" si="3"/>
-        <v>0.88916</v>
+        <v>0.841568</v>
       </c>
       <c r="AD12" s="29">
         <f t="shared" si="3"/>
-        <v>1.19388</v>
+        <v>1.071096</v>
       </c>
       <c r="AE12" s="29">
         <f t="shared" si="3"/>
-        <v>0.859128</v>
+        <v>1.095736</v>
       </c>
       <c r="AF12" s="29">
         <f t="shared" si="3"/>
-        <v>1.105696</v>
+        <v>0.981528</v>
       </c>
       <c r="AG12" s="29">
         <f t="shared" si="3"/>
-        <v>1.159464</v>
+        <v>1.043536</v>
       </c>
       <c r="AH12" s="29">
         <f t="shared" si="3"/>
-        <v>1.194608</v>
+        <v>1.139568</v>
       </c>
       <c r="AI12" s="29">
         <f t="shared" si="3"/>
-        <v>1.07128</v>
+        <v>1.083016</v>
       </c>
       <c r="AJ12" s="29">
         <f t="shared" si="3"/>
-        <v>1.189224</v>
+        <v>1.014496</v>
       </c>
       <c r="AK12" s="29">
         <f t="shared" si="3"/>
-        <v>1.031616</v>
+        <v>0.848352</v>
       </c>
       <c r="AL12" s="29">
         <f t="shared" si="3"/>
-        <v>1.05992</v>
+        <v>1.178808</v>
       </c>
       <c r="AM12" s="29">
         <f t="shared" si="3"/>
-        <v>1.032752</v>
+        <v>1.152352</v>
       </c>
       <c r="AN12" s="29">
         <f t="shared" si="3"/>
-        <v>1.164168</v>
+        <v>1.119024</v>
       </c>
       <c r="AO12" s="29">
         <f t="shared" si="3"/>
-        <v>1.06944</v>
+        <v>0.968832</v>
       </c>
       <c r="AP12" s="29">
         <f t="shared" si="3"/>
-        <v>0.816912</v>
+        <v>1.13808</v>
       </c>
       <c r="AQ12" s="29">
         <f t="shared" si="3"/>
-        <v>0.842568</v>
+        <v>1.0568</v>
       </c>
       <c r="AR12" s="29">
         <f t="shared" si="3"/>
-        <v>1.02176</v>
+        <v>0.965176</v>
       </c>
       <c r="AS12" s="29">
         <f t="shared" si="3"/>
-        <v>1.020064</v>
+        <v>0.974416</v>
       </c>
       <c r="AT12" s="29">
         <f t="shared" si="3"/>
-        <v>0.972936</v>
+        <v>1.077544</v>
       </c>
       <c r="AU12" s="29">
         <f t="shared" si="3"/>
-        <v>0.925224</v>
+        <v>0.850968</v>
       </c>
       <c r="AV12" s="29">
         <f t="shared" si="3"/>
-        <v>1.157464</v>
+        <v>1.100704</v>
       </c>
       <c r="AW12" s="29">
         <f t="shared" si="3"/>
-        <v>0.89444</v>
+        <v>0.980016</v>
       </c>
       <c r="AX12" s="29">
         <f t="shared" si="3"/>
-        <v>1.017144</v>
+        <v>1.158464</v>
       </c>
       <c r="AY12" s="29">
         <f t="shared" si="3"/>
-        <v>0.951696</v>
+        <v>1.028064</v>
       </c>
       <c r="AZ12" s="29">
         <f t="shared" si="3"/>
-        <v>0.893952</v>
+        <v>1.066464</v>
       </c>
       <c r="BA12" s="29">
         <f t="shared" si="3"/>
-        <v>0.92516</v>
+        <v>0.836488</v>
       </c>
       <c r="BB12" s="29">
         <f t="shared" si="3"/>
-        <v>0.958192</v>
+        <v>1.08552</v>
       </c>
       <c r="BC12" s="29">
         <f t="shared" si="3"/>
-        <v>0.824456</v>
+        <v>1.000968</v>
       </c>
       <c r="BD12" s="29">
         <f t="shared" si="3"/>
-        <v>0.941384</v>
+        <v>0.86064</v>
       </c>
       <c r="BE12" s="29">
         <f t="shared" si="3"/>
-        <v>0.957656</v>
+        <v>0.87252</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -2024,7 +2025,7 @@
       </c>
       <c r="C13" s="25">
         <f t="array" ref="C13">IF( B14="Short-Term", AVERAGE(F15:BE15)*B15, INDEX(F15:BE15, 1, COUNTA(F15:BE15))*B15 )</f>
-        <v>0.1884175824</v>
+        <v>0.1721401099</v>
       </c>
       <c r="D13" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B14=""Short-Term"", SPARKLINE(F15:BE15,IF(B13=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F15:BE15, 1, COUNTA(F15:BE15)) ,IF(B13=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -2035,211 +2036,211 @@
       </c>
       <c r="F13" s="26">
         <f t="shared" ref="F13:BE13" si="4">RANDBETWEEN(5000,10000)</f>
-        <v>9448</v>
+        <v>7041</v>
       </c>
       <c r="G13" s="26">
         <f t="shared" si="4"/>
-        <v>9372</v>
+        <v>9016</v>
       </c>
       <c r="H13" s="26">
         <f t="shared" si="4"/>
-        <v>7850</v>
+        <v>9099</v>
       </c>
       <c r="I13" s="26">
         <f t="shared" si="4"/>
-        <v>7421</v>
+        <v>9736</v>
       </c>
       <c r="J13" s="26">
         <f t="shared" si="4"/>
-        <v>5097</v>
+        <v>6696</v>
       </c>
       <c r="K13" s="26">
         <f t="shared" si="4"/>
-        <v>8619</v>
+        <v>6587</v>
       </c>
       <c r="L13" s="26">
         <f t="shared" si="4"/>
-        <v>7429</v>
+        <v>5786</v>
       </c>
       <c r="M13" s="26">
         <f t="shared" si="4"/>
-        <v>6013</v>
+        <v>7236</v>
       </c>
       <c r="N13" s="26">
         <f t="shared" si="4"/>
-        <v>7130</v>
+        <v>6195</v>
       </c>
       <c r="O13" s="26">
         <f t="shared" si="4"/>
-        <v>5842</v>
+        <v>5250</v>
       </c>
       <c r="P13" s="26">
         <f t="shared" si="4"/>
-        <v>6443</v>
+        <v>9278</v>
       </c>
       <c r="Q13" s="26">
         <f t="shared" si="4"/>
-        <v>6653</v>
+        <v>7463</v>
       </c>
       <c r="R13" s="26">
         <f t="shared" si="4"/>
-        <v>8971</v>
+        <v>9817</v>
       </c>
       <c r="S13" s="26">
         <f t="shared" si="4"/>
-        <v>6209</v>
+        <v>8709</v>
       </c>
       <c r="T13" s="26">
         <f t="shared" si="4"/>
-        <v>6286</v>
+        <v>7971</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="4"/>
-        <v>6928</v>
+        <v>8897</v>
       </c>
       <c r="V13" s="26">
         <f t="shared" si="4"/>
-        <v>7334</v>
+        <v>6874</v>
       </c>
       <c r="W13" s="26">
         <f t="shared" si="4"/>
-        <v>8825</v>
+        <v>9848</v>
       </c>
       <c r="X13" s="26">
         <f t="shared" si="4"/>
-        <v>6644</v>
+        <v>7674</v>
       </c>
       <c r="Y13" s="26">
         <f t="shared" si="4"/>
-        <v>9802</v>
+        <v>7191</v>
       </c>
       <c r="Z13" s="26">
         <f t="shared" si="4"/>
-        <v>7633</v>
+        <v>8311</v>
       </c>
       <c r="AA13" s="26">
         <f t="shared" si="4"/>
-        <v>6931</v>
+        <v>8946</v>
       </c>
       <c r="AB13" s="26">
         <f t="shared" si="4"/>
-        <v>6873</v>
+        <v>7192</v>
       </c>
       <c r="AC13" s="26">
         <f t="shared" si="4"/>
-        <v>6916</v>
+        <v>8533</v>
       </c>
       <c r="AD13" s="26">
         <f t="shared" si="4"/>
-        <v>7548</v>
+        <v>6587</v>
       </c>
       <c r="AE13" s="26">
         <f t="shared" si="4"/>
-        <v>5826</v>
+        <v>6629</v>
       </c>
       <c r="AF13" s="26">
         <f t="shared" si="4"/>
-        <v>5657</v>
+        <v>8802</v>
       </c>
       <c r="AG13" s="26">
         <f t="shared" si="4"/>
-        <v>9210</v>
+        <v>9852</v>
       </c>
       <c r="AH13" s="26">
         <f t="shared" si="4"/>
-        <v>9334</v>
+        <v>5993</v>
       </c>
       <c r="AI13" s="26">
         <f t="shared" si="4"/>
-        <v>6861</v>
+        <v>8308</v>
       </c>
       <c r="AJ13" s="26">
         <f t="shared" si="4"/>
-        <v>7869</v>
+        <v>6479</v>
       </c>
       <c r="AK13" s="26">
         <f t="shared" si="4"/>
-        <v>7476</v>
+        <v>9998</v>
       </c>
       <c r="AL13" s="26">
         <f t="shared" si="4"/>
-        <v>6308</v>
+        <v>7955</v>
       </c>
       <c r="AM13" s="26">
         <f t="shared" si="4"/>
-        <v>6598</v>
+        <v>9096</v>
       </c>
       <c r="AN13" s="26">
         <f t="shared" si="4"/>
-        <v>9401</v>
+        <v>9736</v>
       </c>
       <c r="AO13" s="26">
         <f t="shared" si="4"/>
-        <v>6265</v>
+        <v>8979</v>
       </c>
       <c r="AP13" s="26">
         <f t="shared" si="4"/>
-        <v>9023</v>
+        <v>9731</v>
       </c>
       <c r="AQ13" s="26">
         <f t="shared" si="4"/>
-        <v>7336</v>
+        <v>8218</v>
       </c>
       <c r="AR13" s="26">
         <f t="shared" si="4"/>
-        <v>5235</v>
+        <v>9860</v>
       </c>
       <c r="AS13" s="26">
         <f t="shared" si="4"/>
-        <v>9215</v>
+        <v>5555</v>
       </c>
       <c r="AT13" s="26">
         <f t="shared" si="4"/>
-        <v>6801</v>
+        <v>5134</v>
       </c>
       <c r="AU13" s="26">
         <f t="shared" si="4"/>
-        <v>8705</v>
+        <v>9516</v>
       </c>
       <c r="AV13" s="26">
         <f t="shared" si="4"/>
-        <v>8160</v>
+        <v>8137</v>
       </c>
       <c r="AW13" s="26">
         <f t="shared" si="4"/>
-        <v>7504</v>
+        <v>6783</v>
       </c>
       <c r="AX13" s="26">
         <f t="shared" si="4"/>
-        <v>5721</v>
+        <v>7567</v>
       </c>
       <c r="AY13" s="26">
         <f t="shared" si="4"/>
-        <v>9981</v>
+        <v>9929</v>
       </c>
       <c r="AZ13" s="26">
         <f t="shared" si="4"/>
-        <v>5370</v>
+        <v>7397</v>
       </c>
       <c r="BA13" s="26">
         <f t="shared" si="4"/>
-        <v>5625</v>
+        <v>6607</v>
       </c>
       <c r="BB13" s="26">
         <f t="shared" si="4"/>
-        <v>9571</v>
+        <v>8693</v>
       </c>
       <c r="BC13" s="26">
         <f t="shared" si="4"/>
-        <v>9094</v>
+        <v>5793</v>
       </c>
       <c r="BD13" s="26">
         <f t="shared" si="4"/>
-        <v>7637</v>
+        <v>8808</v>
       </c>
       <c r="BE13" s="26">
         <f t="shared" si="4"/>
-        <v>5080</v>
+        <v>9217</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
@@ -2418,211 +2419,211 @@
       </c>
       <c r="F15" s="29">
         <f t="shared" ref="F15:BE15" si="5">IF( $B13="Maximum", F13/F14 , IF( 100%-(F13-F14)/F14 &gt; 0, 100%-(F13-F14)/F14, 0) )</f>
-        <v>0.6502857143</v>
+        <v>0.9941428571</v>
       </c>
       <c r="G15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6611428571</v>
+        <v>0.712</v>
       </c>
       <c r="H15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8785714286</v>
+        <v>0.7001428571</v>
       </c>
       <c r="I15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9398571429</v>
+        <v>0.6091428571</v>
       </c>
       <c r="J15" s="29">
         <f t="shared" si="5"/>
-        <v>1.271857143</v>
+        <v>1.043428571</v>
       </c>
       <c r="K15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7687142857</v>
+        <v>1.059</v>
       </c>
       <c r="L15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9387142857</v>
+        <v>1.173428571</v>
       </c>
       <c r="M15" s="29">
         <f t="shared" si="5"/>
-        <v>1.141</v>
+        <v>0.9662857143</v>
       </c>
       <c r="N15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9814285714</v>
+        <v>1.115</v>
       </c>
       <c r="O15" s="29">
         <f t="shared" si="5"/>
-        <v>1.165428571</v>
+        <v>1.25</v>
       </c>
       <c r="P15" s="29">
         <f t="shared" si="5"/>
-        <v>1.079571429</v>
+        <v>0.6745714286</v>
       </c>
       <c r="Q15" s="29">
         <f t="shared" si="5"/>
-        <v>1.049571429</v>
+        <v>0.9338571429</v>
       </c>
       <c r="R15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7184285714</v>
+        <v>0.5975714286</v>
       </c>
       <c r="S15" s="29">
         <f t="shared" si="5"/>
-        <v>1.113</v>
+        <v>0.7558571429</v>
       </c>
       <c r="T15" s="29">
         <f t="shared" si="5"/>
-        <v>1.102</v>
+        <v>0.8612857143</v>
       </c>
       <c r="U15" s="29">
         <f t="shared" si="5"/>
-        <v>1.010285714</v>
+        <v>0.729</v>
       </c>
       <c r="V15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9522857143</v>
+        <v>1.018</v>
       </c>
       <c r="W15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7392857143</v>
+        <v>0.5931428571</v>
       </c>
       <c r="X15" s="29">
         <f t="shared" si="5"/>
-        <v>1.050857143</v>
+        <v>0.9037142857</v>
       </c>
       <c r="Y15" s="29">
         <f t="shared" si="5"/>
-        <v>0.5997142857</v>
+        <v>0.9727142857</v>
       </c>
       <c r="Z15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9095714286</v>
+        <v>0.8127142857</v>
       </c>
       <c r="AA15" s="29">
         <f t="shared" si="5"/>
-        <v>1.009857143</v>
+        <v>0.722</v>
       </c>
       <c r="AB15" s="29">
         <f t="shared" si="5"/>
-        <v>1.018142857</v>
+        <v>0.9725714286</v>
       </c>
       <c r="AC15" s="29">
         <f t="shared" si="5"/>
-        <v>1.012</v>
+        <v>0.781</v>
       </c>
       <c r="AD15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9217142857</v>
+        <v>1.059</v>
       </c>
       <c r="AE15" s="29">
         <f t="shared" si="5"/>
-        <v>1.167714286</v>
+        <v>1.053</v>
       </c>
       <c r="AF15" s="29">
         <f t="shared" si="5"/>
-        <v>1.191857143</v>
+        <v>0.7425714286</v>
       </c>
       <c r="AG15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6842857143</v>
+        <v>0.5925714286</v>
       </c>
       <c r="AH15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6665714286</v>
+        <v>1.143857143</v>
       </c>
       <c r="AI15" s="29">
         <f t="shared" si="5"/>
-        <v>1.019857143</v>
+        <v>0.8131428571</v>
       </c>
       <c r="AJ15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8758571429</v>
+        <v>1.074428571</v>
       </c>
       <c r="AK15" s="29">
         <f t="shared" si="5"/>
-        <v>0.932</v>
+        <v>0.5717142857</v>
       </c>
       <c r="AL15" s="29">
         <f t="shared" si="5"/>
-        <v>1.098857143</v>
+        <v>0.8635714286</v>
       </c>
       <c r="AM15" s="29">
         <f t="shared" si="5"/>
-        <v>1.057428571</v>
+        <v>0.7005714286</v>
       </c>
       <c r="AN15" s="29">
         <f t="shared" si="5"/>
-        <v>0.657</v>
+        <v>0.6091428571</v>
       </c>
       <c r="AO15" s="29">
         <f t="shared" si="5"/>
-        <v>1.105</v>
+        <v>0.7172857143</v>
       </c>
       <c r="AP15" s="29">
         <f t="shared" si="5"/>
-        <v>0.711</v>
+        <v>0.6098571429</v>
       </c>
       <c r="AQ15" s="29">
         <f t="shared" si="5"/>
-        <v>0.952</v>
+        <v>0.826</v>
       </c>
       <c r="AR15" s="29">
         <f t="shared" si="5"/>
-        <v>1.252142857</v>
+        <v>0.5914285714</v>
       </c>
       <c r="AS15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6835714286</v>
+        <v>1.206428571</v>
       </c>
       <c r="AT15" s="29">
         <f t="shared" si="5"/>
-        <v>1.028428571</v>
+        <v>1.266571429</v>
       </c>
       <c r="AU15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7564285714</v>
+        <v>0.6405714286</v>
       </c>
       <c r="AV15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8342857143</v>
+        <v>0.8375714286</v>
       </c>
       <c r="AW15" s="29">
         <f t="shared" si="5"/>
-        <v>0.928</v>
+        <v>1.031</v>
       </c>
       <c r="AX15" s="29">
         <f t="shared" si="5"/>
-        <v>1.182714286</v>
+        <v>0.919</v>
       </c>
       <c r="AY15" s="29">
         <f t="shared" si="5"/>
-        <v>0.5741428571</v>
+        <v>0.5815714286</v>
       </c>
       <c r="AZ15" s="29">
         <f t="shared" si="5"/>
-        <v>1.232857143</v>
+        <v>0.9432857143</v>
       </c>
       <c r="BA15" s="29">
         <f t="shared" si="5"/>
-        <v>1.196428571</v>
+        <v>1.056142857</v>
       </c>
       <c r="BB15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6327142857</v>
+        <v>0.7581428571</v>
       </c>
       <c r="BC15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7008571429</v>
+        <v>1.172428571</v>
       </c>
       <c r="BD15" s="29">
         <f t="shared" si="5"/>
-        <v>0.909</v>
+        <v>0.7417142857</v>
       </c>
       <c r="BE15" s="29">
         <f t="shared" si="5"/>
-        <v>1.274285714</v>
+        <v>0.6832857143</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -4398,7 +4399,7 @@
       <c r="B30" s="19"/>
       <c r="C30" s="20">
         <f>SUMIFS(C31:C1013,A31:A1013,A31)</f>
-        <v>0.6844230769</v>
+        <v>0.7033269231</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
@@ -4464,7 +4465,7 @@
       </c>
       <c r="C31" s="25">
         <f t="array" ref="C31">IF( B32="Short-Term", AVERAGE(F33:BE33)*B33, INDEX(F33:BE33, 1, COUNTA(F33:BE33))*B33 )</f>
-        <v>0.3298076923</v>
+        <v>0.3470384615</v>
       </c>
       <c r="D31" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B32=""Short-Term"", SPARKLINE(F33:BE33,IF(B31=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F33:BE33, 1, COUNTA(F33:BE33)) ,IF(B31=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -4475,95 +4476,95 @@
       </c>
       <c r="F31" s="26">
         <f t="shared" ref="F31:BE31" si="9">RANDBETWEEN(1,50)</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G31" s="26">
         <f t="shared" si="9"/>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H31" s="26">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I31" s="26">
         <f t="shared" si="9"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J31" s="26">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="K31" s="26">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L31" s="26">
         <f t="shared" si="9"/>
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M31" s="26">
         <f t="shared" si="9"/>
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="N31" s="26">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="O31" s="26">
         <f t="shared" si="9"/>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="P31" s="26">
         <f t="shared" si="9"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q31" s="26">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="R31" s="26">
         <f t="shared" si="9"/>
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="S31" s="26">
         <f t="shared" si="9"/>
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="T31" s="26">
         <f t="shared" si="9"/>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="U31" s="26">
         <f t="shared" si="9"/>
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="V31" s="26">
         <f t="shared" si="9"/>
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="W31" s="26">
         <f t="shared" si="9"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="X31" s="26">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="Y31" s="26">
         <f t="shared" si="9"/>
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="Z31" s="26">
         <f t="shared" si="9"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AA31" s="26">
         <f t="shared" si="9"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AB31" s="26">
         <f t="shared" si="9"/>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="AC31" s="26">
         <f t="shared" si="9"/>
@@ -4571,79 +4572,79 @@
       </c>
       <c r="AD31" s="26">
         <f t="shared" si="9"/>
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="AE31" s="26">
         <f t="shared" si="9"/>
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="AF31" s="26">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="AG31" s="26">
         <f t="shared" si="9"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AH31" s="26">
         <f t="shared" si="9"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="AI31" s="26">
         <f t="shared" si="9"/>
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="AJ31" s="26">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="AK31" s="26">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="AL31" s="26">
         <f t="shared" si="9"/>
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="AM31" s="26">
         <f t="shared" si="9"/>
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="AN31" s="26">
         <f t="shared" si="9"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="AO31" s="26">
         <f t="shared" si="9"/>
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="AP31" s="26">
         <f t="shared" si="9"/>
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="AQ31" s="26">
         <f t="shared" si="9"/>
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="AR31" s="26">
         <f t="shared" si="9"/>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="AS31" s="26">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="AT31" s="26">
         <f t="shared" si="9"/>
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="AU31" s="26">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="AV31" s="26">
         <f t="shared" si="9"/>
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="AW31" s="26">
         <f t="shared" si="9"/>
@@ -4651,15 +4652,15 @@
       </c>
       <c r="AX31" s="26">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="AY31" s="26">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="AZ31" s="26">
         <f t="shared" si="9"/>
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="BA31" s="26">
         <f t="shared" si="9"/>
@@ -4667,19 +4668,19 @@
       </c>
       <c r="BB31" s="26">
         <f t="shared" si="9"/>
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="BC31" s="26">
         <f t="shared" si="9"/>
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="BD31" s="26">
         <f t="shared" si="9"/>
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="BE31" s="26">
         <f t="shared" si="9"/>
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -4858,95 +4859,95 @@
       </c>
       <c r="F33" s="29">
         <f t="shared" ref="F33:BE33" si="10">IF( $B31="Maximum", F31/F32 , IF( 100%-(F31-F32)/F32 &gt; 0, 100%-(F31-F32)/F32, 0) )</f>
-        <v>0.22</v>
+        <v>0.12</v>
       </c>
       <c r="G33" s="29">
         <f t="shared" si="10"/>
-        <v>0.42</v>
+        <v>0.48</v>
       </c>
       <c r="H33" s="29">
         <f t="shared" si="10"/>
-        <v>0.18</v>
+        <v>0.1</v>
       </c>
       <c r="I33" s="29">
         <f t="shared" si="10"/>
-        <v>0.4</v>
+        <v>0.34</v>
       </c>
       <c r="J33" s="29">
         <f t="shared" si="10"/>
-        <v>0.26</v>
+        <v>0.96</v>
       </c>
       <c r="K33" s="29">
         <f t="shared" si="10"/>
-        <v>0.12</v>
+        <v>0.04</v>
       </c>
       <c r="L33" s="29">
         <f t="shared" si="10"/>
-        <v>0.54</v>
+        <v>0.48</v>
       </c>
       <c r="M33" s="29">
         <f t="shared" si="10"/>
-        <v>0.68</v>
+        <v>0.9</v>
       </c>
       <c r="N33" s="29">
         <f t="shared" si="10"/>
-        <v>0.28</v>
+        <v>0.94</v>
       </c>
       <c r="O33" s="29">
         <f t="shared" si="10"/>
-        <v>0.32</v>
+        <v>0.62</v>
       </c>
       <c r="P33" s="29">
         <f t="shared" si="10"/>
-        <v>0.34</v>
+        <v>0.24</v>
       </c>
       <c r="Q33" s="29">
         <f t="shared" si="10"/>
-        <v>0.28</v>
+        <v>0.38</v>
       </c>
       <c r="R33" s="29">
         <f t="shared" si="10"/>
-        <v>0.48</v>
+        <v>0.08</v>
       </c>
       <c r="S33" s="29">
         <f t="shared" si="10"/>
-        <v>0.7</v>
+        <v>0.06</v>
       </c>
       <c r="T33" s="29">
         <f t="shared" si="10"/>
-        <v>0.34</v>
+        <v>0.22</v>
       </c>
       <c r="U33" s="29">
         <f t="shared" si="10"/>
-        <v>0.9</v>
+        <v>0.06</v>
       </c>
       <c r="V33" s="29">
         <f t="shared" si="10"/>
-        <v>0.52</v>
+        <v>0.12</v>
       </c>
       <c r="W33" s="29">
         <f t="shared" si="10"/>
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
       <c r="X33" s="29">
         <f t="shared" si="10"/>
-        <v>0.18</v>
+        <v>0.46</v>
       </c>
       <c r="Y33" s="29">
         <f t="shared" si="10"/>
-        <v>0.52</v>
+        <v>0.86</v>
       </c>
       <c r="Z33" s="29">
         <f t="shared" si="10"/>
-        <v>0.74</v>
+        <v>0.7</v>
       </c>
       <c r="AA33" s="29">
         <f t="shared" si="10"/>
-        <v>0.74</v>
+        <v>0.72</v>
       </c>
       <c r="AB33" s="29">
         <f t="shared" si="10"/>
-        <v>0.56</v>
+        <v>0.5</v>
       </c>
       <c r="AC33" s="29">
         <f t="shared" si="10"/>
@@ -4954,79 +4955,79 @@
       </c>
       <c r="AD33" s="29">
         <f t="shared" si="10"/>
-        <v>0.38</v>
+        <v>1</v>
       </c>
       <c r="AE33" s="29">
         <f t="shared" si="10"/>
-        <v>0.46</v>
+        <v>0.78</v>
       </c>
       <c r="AF33" s="29">
         <f t="shared" si="10"/>
-        <v>0.02</v>
+        <v>0.64</v>
       </c>
       <c r="AG33" s="29">
         <f t="shared" si="10"/>
-        <v>0.54</v>
+        <v>0.56</v>
       </c>
       <c r="AH33" s="29">
         <f t="shared" si="10"/>
-        <v>0.44</v>
+        <v>0.5</v>
       </c>
       <c r="AI33" s="29">
         <f t="shared" si="10"/>
-        <v>0.96</v>
+        <v>0.76</v>
       </c>
       <c r="AJ33" s="29">
         <f t="shared" si="10"/>
-        <v>0.08</v>
+        <v>0.76</v>
       </c>
       <c r="AK33" s="29">
         <f t="shared" si="10"/>
-        <v>0.18</v>
+        <v>0.56</v>
       </c>
       <c r="AL33" s="29">
         <f t="shared" si="10"/>
-        <v>0.78</v>
+        <v>0.86</v>
       </c>
       <c r="AM33" s="29">
         <f t="shared" si="10"/>
-        <v>0.62</v>
+        <v>0.46</v>
       </c>
       <c r="AN33" s="29">
         <f t="shared" si="10"/>
-        <v>0.32</v>
+        <v>0.12</v>
       </c>
       <c r="AO33" s="29">
         <f t="shared" si="10"/>
-        <v>0.54</v>
+        <v>0.38</v>
       </c>
       <c r="AP33" s="29">
         <f t="shared" si="10"/>
-        <v>0.42</v>
+        <v>0.94</v>
       </c>
       <c r="AQ33" s="29">
         <f t="shared" si="10"/>
-        <v>0.82</v>
+        <v>0.58</v>
       </c>
       <c r="AR33" s="29">
         <f t="shared" si="10"/>
-        <v>0.32</v>
+        <v>0.06</v>
       </c>
       <c r="AS33" s="29">
         <f t="shared" si="10"/>
-        <v>0.28</v>
+        <v>0.78</v>
       </c>
       <c r="AT33" s="29">
         <f t="shared" si="10"/>
-        <v>0.54</v>
+        <v>0.14</v>
       </c>
       <c r="AU33" s="29">
         <f t="shared" si="10"/>
-        <v>0.06</v>
+        <v>0.4</v>
       </c>
       <c r="AV33" s="29">
         <f t="shared" si="10"/>
-        <v>0.88</v>
+        <v>0.7</v>
       </c>
       <c r="AW33" s="29">
         <f t="shared" si="10"/>
@@ -5034,15 +5035,15 @@
       </c>
       <c r="AX33" s="29">
         <f t="shared" si="10"/>
-        <v>0.28</v>
+        <v>0.62</v>
       </c>
       <c r="AY33" s="29">
         <f t="shared" si="10"/>
-        <v>0.1</v>
+        <v>0.86</v>
       </c>
       <c r="AZ33" s="29">
         <f t="shared" si="10"/>
-        <v>0.98</v>
+        <v>0.6</v>
       </c>
       <c r="BA33" s="29">
         <f t="shared" si="10"/>
@@ -5050,19 +5051,19 @@
       </c>
       <c r="BB33" s="29">
         <f t="shared" si="10"/>
-        <v>0.74</v>
+        <v>0.08</v>
       </c>
       <c r="BC33" s="29">
         <f t="shared" si="10"/>
-        <v>0.98</v>
+        <v>0.82</v>
       </c>
       <c r="BD33" s="29">
         <f t="shared" si="10"/>
-        <v>0.84</v>
+        <v>0.44</v>
       </c>
       <c r="BE33" s="29">
         <f t="shared" si="10"/>
-        <v>0.48</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -5074,7 +5075,7 @@
       </c>
       <c r="C34" s="25">
         <f t="array" ref="C34">IF( B35="Short-Term", AVERAGE(F36:BE36)*B36, INDEX(F36:BE36, 1, COUNTA(F36:BE36))*B36 )</f>
-        <v>0.02346153846</v>
+        <v>0.02513461538</v>
       </c>
       <c r="D34" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B35=""Short-Term"", SPARKLINE(F36:BE36,IF(B34=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F36:BE36, 1, COUNTA(F36:BE36)) ,IF(B34=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -5085,211 +5086,211 @@
       </c>
       <c r="F34" s="26">
         <f t="shared" ref="F34:BE34" si="11">RANDBETWEEN(1,50)</f>
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G34" s="26">
         <f t="shared" si="11"/>
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="H34" s="26">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I34" s="26">
         <f t="shared" si="11"/>
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="J34" s="26">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K34" s="26">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="L34" s="26">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="M34" s="26">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="N34" s="26">
         <f t="shared" si="11"/>
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="O34" s="26">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="P34" s="26">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="Q34" s="26">
         <f t="shared" si="11"/>
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="R34" s="26">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="S34" s="26">
         <f t="shared" si="11"/>
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="T34" s="26">
         <f t="shared" si="11"/>
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="U34" s="26">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="V34" s="26">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="W34" s="26">
         <f t="shared" si="11"/>
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="X34" s="26">
         <f t="shared" si="11"/>
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="Y34" s="26">
         <f t="shared" si="11"/>
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="Z34" s="26">
         <f t="shared" si="11"/>
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="AA34" s="26">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="AB34" s="26">
         <f t="shared" si="11"/>
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="AC34" s="26">
         <f t="shared" si="11"/>
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AD34" s="26">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="AE34" s="26">
         <f t="shared" si="11"/>
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="AF34" s="26">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG34" s="26">
         <f t="shared" si="11"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="AH34" s="26">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="AI34" s="26">
         <f t="shared" si="11"/>
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="AJ34" s="26">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="AK34" s="26">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="AL34" s="26">
         <f t="shared" si="11"/>
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="AM34" s="26">
         <f t="shared" si="11"/>
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="AN34" s="26">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="AO34" s="26">
         <f t="shared" si="11"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AP34" s="26">
         <f t="shared" si="11"/>
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="AQ34" s="26">
         <f t="shared" si="11"/>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AR34" s="26">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="AS34" s="26">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="AT34" s="26">
         <f t="shared" si="11"/>
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="AU34" s="26">
         <f t="shared" si="11"/>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="AV34" s="26">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AW34" s="26">
         <f t="shared" si="11"/>
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="AX34" s="26">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="AY34" s="26">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AZ34" s="26">
         <f t="shared" si="11"/>
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="BA34" s="26">
         <f t="shared" si="11"/>
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="BB34" s="26">
         <f t="shared" si="11"/>
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="BC34" s="26">
         <f t="shared" si="11"/>
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="BD34" s="26">
         <f t="shared" si="11"/>
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="BE34" s="26">
         <f t="shared" si="11"/>
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -5468,211 +5469,211 @@
       </c>
       <c r="F36" s="29">
         <f t="shared" ref="F36:BE36" si="12">IF( $B34="Maximum", F34/F35 , IF( 100%-(F34-F35)/F35 &gt; 0, 100%-(F34-F35)/F35, 0) )</f>
-        <v>0.09</v>
+        <v>0.22</v>
       </c>
       <c r="G36" s="29">
         <f t="shared" si="12"/>
-        <v>0.39</v>
+        <v>0.29</v>
       </c>
       <c r="H36" s="29">
         <f t="shared" si="12"/>
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="I36" s="29">
         <f t="shared" si="12"/>
-        <v>0.37</v>
+        <v>0.45</v>
       </c>
       <c r="J36" s="29">
         <f t="shared" si="12"/>
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="K36" s="29">
         <f t="shared" si="12"/>
-        <v>0.4</v>
+        <v>0.03</v>
       </c>
       <c r="L36" s="29">
         <f t="shared" si="12"/>
-        <v>0.1</v>
+        <v>0.32</v>
       </c>
       <c r="M36" s="29">
         <f t="shared" si="12"/>
-        <v>0.04</v>
+        <v>0.28</v>
       </c>
       <c r="N36" s="29">
         <f t="shared" si="12"/>
-        <v>0.33</v>
+        <v>0.01</v>
       </c>
       <c r="O36" s="29">
         <f t="shared" si="12"/>
-        <v>0.02</v>
+        <v>0.17</v>
       </c>
       <c r="P36" s="29">
         <f t="shared" si="12"/>
-        <v>0.04</v>
+        <v>0.4</v>
       </c>
       <c r="Q36" s="29">
         <f t="shared" si="12"/>
-        <v>0.49</v>
+        <v>0.11</v>
       </c>
       <c r="R36" s="29">
         <f t="shared" si="12"/>
-        <v>0.02</v>
+        <v>0.41</v>
       </c>
       <c r="S36" s="29">
         <f t="shared" si="12"/>
-        <v>0.27</v>
+        <v>0.32</v>
       </c>
       <c r="T36" s="29">
         <f t="shared" si="12"/>
-        <v>0.33</v>
+        <v>0.39</v>
       </c>
       <c r="U36" s="29">
         <f t="shared" si="12"/>
-        <v>0.01</v>
+        <v>0.3</v>
       </c>
       <c r="V36" s="29">
         <f t="shared" si="12"/>
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="W36" s="29">
         <f t="shared" si="12"/>
-        <v>0.42</v>
+        <v>0.2</v>
       </c>
       <c r="X36" s="29">
         <f t="shared" si="12"/>
-        <v>0.45</v>
+        <v>0.41</v>
       </c>
       <c r="Y36" s="29">
         <f t="shared" si="12"/>
-        <v>0.25</v>
+        <v>0.16</v>
       </c>
       <c r="Z36" s="29">
         <f t="shared" si="12"/>
-        <v>0.22</v>
+        <v>0.46</v>
       </c>
       <c r="AA36" s="29">
         <f t="shared" si="12"/>
-        <v>0.15</v>
+        <v>0.09</v>
       </c>
       <c r="AB36" s="29">
         <f t="shared" si="12"/>
-        <v>0.41</v>
+        <v>0.48</v>
       </c>
       <c r="AC36" s="29">
         <f t="shared" si="12"/>
-        <v>0.25</v>
+        <v>0.17</v>
       </c>
       <c r="AD36" s="29">
         <f t="shared" si="12"/>
-        <v>0.04</v>
+        <v>0.31</v>
       </c>
       <c r="AE36" s="29">
         <f t="shared" si="12"/>
-        <v>0.28</v>
+        <v>0.41</v>
       </c>
       <c r="AF36" s="29">
         <f t="shared" si="12"/>
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="AG36" s="29">
         <f t="shared" si="12"/>
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
       <c r="AH36" s="29">
         <f t="shared" si="12"/>
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="AI36" s="29">
         <f t="shared" si="12"/>
-        <v>0.17</v>
+        <v>0.45</v>
       </c>
       <c r="AJ36" s="29">
         <f t="shared" si="12"/>
-        <v>0.02</v>
+        <v>0.09</v>
       </c>
       <c r="AK36" s="29">
         <f t="shared" si="12"/>
-        <v>0.13</v>
+        <v>0.39</v>
       </c>
       <c r="AL36" s="29">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.37</v>
       </c>
       <c r="AM36" s="29">
         <f t="shared" si="12"/>
-        <v>0.19</v>
+        <v>0.35</v>
       </c>
       <c r="AN36" s="29">
         <f t="shared" si="12"/>
-        <v>0.3</v>
+        <v>0.11</v>
       </c>
       <c r="AO36" s="29">
         <f t="shared" si="12"/>
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="AP36" s="29">
         <f t="shared" si="12"/>
-        <v>0.27</v>
+        <v>0.21</v>
       </c>
       <c r="AQ36" s="29">
         <f t="shared" si="12"/>
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="AR36" s="29">
         <f t="shared" si="12"/>
-        <v>0.3</v>
+        <v>0.39</v>
       </c>
       <c r="AS36" s="29">
         <f t="shared" si="12"/>
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="AT36" s="29">
         <f t="shared" si="12"/>
-        <v>0.21</v>
+        <v>0.09</v>
       </c>
       <c r="AU36" s="29">
         <f t="shared" si="12"/>
-        <v>0.36</v>
+        <v>0.28</v>
       </c>
       <c r="AV36" s="29">
         <f t="shared" si="12"/>
-        <v>0.01</v>
+        <v>0.09</v>
       </c>
       <c r="AW36" s="29">
         <f t="shared" si="12"/>
-        <v>0.37</v>
+        <v>0.25</v>
       </c>
       <c r="AX36" s="29">
         <f t="shared" si="12"/>
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
       <c r="AY36" s="29">
         <f t="shared" si="12"/>
-        <v>0.06</v>
+        <v>0.15</v>
       </c>
       <c r="AZ36" s="29">
         <f t="shared" si="12"/>
-        <v>0.43</v>
+        <v>0.26</v>
       </c>
       <c r="BA36" s="29">
         <f t="shared" si="12"/>
-        <v>0.31</v>
+        <v>0.06</v>
       </c>
       <c r="BB36" s="29">
         <f t="shared" si="12"/>
-        <v>0.22</v>
+        <v>0.33</v>
       </c>
       <c r="BC36" s="29">
         <f t="shared" si="12"/>
-        <v>0.28</v>
+        <v>0.05</v>
       </c>
       <c r="BD36" s="29">
         <f t="shared" si="12"/>
-        <v>0.49</v>
+        <v>0.27</v>
       </c>
       <c r="BE36" s="29">
         <f t="shared" si="12"/>
-        <v>0.18</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -11206,18 +11207,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:BE10 F13:BE13 F16:BE16 F19:BE19 F25:BE25 F31:BE31 F34:BE34 F37:BE37">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>F11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10:BE10 F13:BE13 F16:BE16 F19:BE19 F25:BE25 F31:BE31 F34:BE34 F37:BE37">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND($B10="Maximum",F10&gt;=F11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:BE10 F13:BE13 F16:BE16 F19:BE19 F25:BE25 F31:BE31 F34:BE34 F37:BE37">
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>AND($B10="Minimum",F10&gt;=F11)</formula>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>AND($B10="Minimum",50%&gt;F12)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:BE10 F13:BE13 F16:BE16 F19:BE19 F25:BE25 F31:BE31 F34:BE34 F37:BE37">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
+      <formula>LEN(TRIM(F10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>

</xml_diff>

<commit_message>
fix: remove unused conditional formatting BSC
</commit_message>
<xml_diff>
--- a/templates/management/Balance Scorecard (BSC).xlsx
+++ b/templates/management/Balance Scorecard (BSC).xlsx
@@ -10,7 +10,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="BERvaqtXSPBSGqlfiskO/Ggi+SOyyx2+IACiiYtFpsU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="GWug7MWjzAta6UaDoivwDwpRKu51o5XpQ53swl4d3UE="/>
     </ext>
   </extLst>
 </workbook>
@@ -82,33 +82,15 @@
 ======</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A32">
-      <text>
-        <t xml:space="preserve">The number of new customers successfully registered for Telkomsel's services.
-======</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="B33">
       <text>
         <t xml:space="preserve">Weight
 ======</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A35">
-      <text>
-        <t xml:space="preserve">The number of new customers successfully registered for Telkomsel's services.
-======</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="B36">
       <text>
         <t xml:space="preserve">Weight
-======</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A38">
-      <text>
-        <t xml:space="preserve">The number of new customers successfully registered for Telkomsel's services.
 ======</t>
       </text>
     </comment>
@@ -146,12 +128,18 @@
 ======</t>
       </text>
     </comment>
+    <comment authorId="0" ref="B20">
+      <text>
+        <t xml:space="preserve">Weight
+======</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="40">
   <si>
     <t>PT. Telkom Indonesia (Persero) Tbk., atau Telkom, adalah Badan Usaha Milik Negara (BUMN) yang bergerak di bidang jasa layanan teknologi informasi dan komunikasi (TIK) dan jaringan telekomunikasi di Indonesia.</t>
   </si>
@@ -210,7 +198,7 @@
     <t>Telkomsel - Pasca Bayar</t>
   </si>
   <si>
-    <t>Maximum</t>
+    <t>Minimum</t>
   </si>
   <si>
     <t>Actual</t>
@@ -228,10 +216,10 @@
     <t>% Target</t>
   </si>
   <si>
-    <t>Minimum</t>
+    <t>Customer Retention (Churn Rate)</t>
   </si>
   <si>
-    <t>Customer Retention (Churn Rate)</t>
+    <t>Maximum</t>
   </si>
   <si>
     <t>Total Revenue</t>
@@ -268,6 +256,9 @@
   </si>
   <si>
     <t>Research Contributions</t>
+  </si>
+  <si>
+    <t>Agung Sundoro</t>
   </si>
 </sst>
 </file>
@@ -441,8 +432,8 @@
       <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
       <border/>
@@ -451,8 +442,8 @@
       <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
       <border/>
@@ -760,211 +751,211 @@
       <c r="E1" s="3"/>
       <c r="F1" s="4">
         <f t="shared" ref="F1:BE1" si="1">AVERAGEIFS(F9:F1013,$E9:$E1013,"% Target")</f>
-        <v>0.4638648736</v>
+        <v>0.5476855879</v>
       </c>
       <c r="G1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4212501978</v>
+        <v>0.4958593407</v>
       </c>
       <c r="H1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4243593571</v>
+        <v>0.3818893571</v>
       </c>
       <c r="I1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5773431319</v>
+        <v>0.575169989</v>
       </c>
       <c r="J1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5991617418</v>
+        <v>0.5814697418</v>
       </c>
       <c r="K1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5606149231</v>
+        <v>0.4971453516</v>
       </c>
       <c r="L1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4173091044</v>
+        <v>0.572833533</v>
       </c>
       <c r="M1" s="4">
         <f t="shared" si="1"/>
-        <v>0.497349</v>
+        <v>0.5798191429</v>
       </c>
       <c r="N1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4693921813</v>
+        <v>0.5578983242</v>
       </c>
       <c r="O1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5918385055</v>
+        <v>0.5489223626</v>
       </c>
       <c r="P1" s="4">
         <f t="shared" si="1"/>
-        <v>0.598028544</v>
+        <v>0.6871329725</v>
       </c>
       <c r="Q1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5604934396</v>
+        <v>0.6182335824</v>
       </c>
       <c r="R1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6210129066</v>
+        <v>0.4932197637</v>
       </c>
       <c r="S1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5318173736</v>
+        <v>0.4935375165</v>
       </c>
       <c r="T1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5642386978</v>
+        <v>0.6285525549</v>
       </c>
       <c r="U1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6157094505</v>
+        <v>0.6043277363</v>
       </c>
       <c r="V1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6886800604</v>
+        <v>0.5898452033</v>
       </c>
       <c r="W1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6462400989</v>
+        <v>0.7299640989</v>
       </c>
       <c r="X1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5834614231</v>
+        <v>0.5666115659</v>
       </c>
       <c r="Y1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5786341758</v>
+        <v>0.606244033</v>
       </c>
       <c r="Z1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7124637857</v>
+        <v>0.6258436429</v>
       </c>
       <c r="AA1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6957811099</v>
+        <v>0.7588926813</v>
       </c>
       <c r="AB1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6757025769</v>
+        <v>0.7149505769</v>
       </c>
       <c r="AC1" s="4">
         <f t="shared" si="1"/>
-        <v>0.717163044</v>
+        <v>0.809738044</v>
       </c>
       <c r="AD1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6517257967</v>
+        <v>0.7316729396</v>
       </c>
       <c r="AE1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7998044066</v>
+        <v>0.7580118352</v>
       </c>
       <c r="AF1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8329143022</v>
+        <v>0.7018445879</v>
       </c>
       <c r="AG1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7211344835</v>
+        <v>0.7790114835</v>
       </c>
       <c r="AH1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8532269505</v>
+        <v>0.7715890934</v>
       </c>
       <c r="AI1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8721604176</v>
+        <v>0.7752677033</v>
       </c>
       <c r="AJ1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8413643132</v>
+        <v>0.7765193132</v>
       </c>
       <c r="AK1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6858274945</v>
+        <v>0.7806887802</v>
       </c>
       <c r="AL1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8837183901</v>
+        <v>0.8285609615</v>
       </c>
       <c r="AM1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8655228571</v>
+        <v>0.8736687143</v>
       </c>
       <c r="AN1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9152473242</v>
+        <v>0.8941190385</v>
       </c>
       <c r="AO1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8816346484</v>
+        <v>0.8578730769</v>
       </c>
       <c r="AP1" s="4">
         <f t="shared" si="1"/>
-        <v>0.914159544</v>
+        <v>0.9002958297</v>
       </c>
       <c r="AQ1" s="4">
         <f t="shared" si="1"/>
-        <v>0.817694011</v>
+        <v>0.8326777253</v>
       </c>
       <c r="AR1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9022257637</v>
+        <v>0.8648131923</v>
       </c>
       <c r="AS1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9331478022</v>
+        <v>0.9090312308</v>
       </c>
       <c r="AT1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9258779835</v>
+        <v>0.9869829835</v>
       </c>
       <c r="AU1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9565327363</v>
+        <v>0.926104022</v>
       </c>
       <c r="AV1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9854900604</v>
+        <v>0.9530286319</v>
       </c>
       <c r="AW1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9118253846</v>
+        <v>0.9556492418</v>
       </c>
       <c r="AX1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8783738516</v>
+        <v>0.9719321374</v>
       </c>
       <c r="AY1" s="4">
         <f t="shared" si="1"/>
-        <v>0.988050033</v>
+        <v>1.07047889</v>
       </c>
       <c r="AZ1" s="4">
         <f t="shared" si="1"/>
-        <v>1.109258357</v>
+        <v>1.112661643</v>
       </c>
       <c r="BA1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9573701099</v>
+        <v>1.071864396</v>
       </c>
       <c r="BB1" s="4">
         <f t="shared" si="1"/>
-        <v>1.048797005</v>
+        <v>1.027063577</v>
       </c>
       <c r="BC1" s="4">
         <f t="shared" si="1"/>
-        <v>1.078631901</v>
+        <v>1.062574187</v>
       </c>
       <c r="BD1" s="4">
         <f t="shared" si="1"/>
-        <v>1.044837082</v>
+        <v>1.063307797</v>
       </c>
       <c r="BE1" s="4">
         <f t="shared" si="1"/>
-        <v>1.079387407</v>
+        <v>1.102497264</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -1420,7 +1411,7 @@
       <c r="B9" s="19"/>
       <c r="C9" s="20">
         <f>SUMIFS(C10:C1013,A10:A1013,A10)</f>
-        <v>0.8890123978</v>
+        <v>0.9026899011</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="22"/>
@@ -1486,7 +1477,7 @@
       </c>
       <c r="C10" s="25">
         <f t="array" ref="C10">IF( B11="Short-Term", AVERAGE(F12:BE12)*B12, INDEX(F12:BE12, 1, COUNTA(F12:BE12))*B12 )</f>
-        <v>0.2994678923</v>
+        <v>0.3030948462</v>
       </c>
       <c r="D10" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B11=""Short-Term"", SPARKLINE(F12:BE12,IF(B10=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F12:BE12, 1, COUNTA(F12:BE12)) ,IF(B10=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -1497,211 +1488,211 @@
       </c>
       <c r="F10" s="26">
         <f t="shared" ref="F10:BE10" si="2">RANDBETWEEN(100000,150000)</f>
-        <v>148176</v>
+        <v>131164</v>
       </c>
       <c r="G10" s="26">
         <f t="shared" si="2"/>
-        <v>100948</v>
+        <v>131550</v>
       </c>
       <c r="H10" s="26">
         <f t="shared" si="2"/>
-        <v>100404</v>
+        <v>145441</v>
       </c>
       <c r="I10" s="26">
         <f t="shared" si="2"/>
-        <v>147475</v>
+        <v>122341</v>
       </c>
       <c r="J10" s="26">
         <f t="shared" si="2"/>
-        <v>127591</v>
+        <v>147101</v>
       </c>
       <c r="K10" s="26">
         <f t="shared" si="2"/>
-        <v>129538</v>
+        <v>130253</v>
       </c>
       <c r="L10" s="26">
         <f t="shared" si="2"/>
-        <v>105976</v>
+        <v>106321</v>
       </c>
       <c r="M10" s="26">
         <f t="shared" si="2"/>
-        <v>149974</v>
+        <v>103413</v>
       </c>
       <c r="N10" s="26">
         <f t="shared" si="2"/>
-        <v>119761</v>
+        <v>112715</v>
       </c>
       <c r="O10" s="26">
         <f t="shared" si="2"/>
-        <v>113969</v>
+        <v>105340</v>
       </c>
       <c r="P10" s="26">
         <f t="shared" si="2"/>
-        <v>134260</v>
+        <v>107207</v>
       </c>
       <c r="Q10" s="26">
         <f t="shared" si="2"/>
-        <v>113433</v>
+        <v>110184</v>
       </c>
       <c r="R10" s="26">
         <f t="shared" si="2"/>
-        <v>139107</v>
+        <v>128704</v>
       </c>
       <c r="S10" s="26">
         <f t="shared" si="2"/>
-        <v>113941</v>
+        <v>116321</v>
       </c>
       <c r="T10" s="26">
         <f t="shared" si="2"/>
-        <v>121249</v>
+        <v>141955</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="2"/>
-        <v>121410</v>
+        <v>119061</v>
       </c>
       <c r="V10" s="26">
         <f t="shared" si="2"/>
-        <v>143553</v>
+        <v>140264</v>
       </c>
       <c r="W10" s="26">
         <f t="shared" si="2"/>
-        <v>145589</v>
+        <v>116562</v>
       </c>
       <c r="X10" s="26">
         <f t="shared" si="2"/>
-        <v>115822</v>
+        <v>123635</v>
       </c>
       <c r="Y10" s="26">
         <f t="shared" si="2"/>
-        <v>124810</v>
+        <v>121473</v>
       </c>
       <c r="Z10" s="26">
         <f t="shared" si="2"/>
-        <v>141062</v>
+        <v>112076</v>
       </c>
       <c r="AA10" s="26">
         <f t="shared" si="2"/>
-        <v>115516</v>
+        <v>123301</v>
       </c>
       <c r="AB10" s="26">
         <f t="shared" si="2"/>
-        <v>119842</v>
+        <v>138785</v>
       </c>
       <c r="AC10" s="26">
         <f t="shared" si="2"/>
-        <v>100207</v>
+        <v>134218</v>
       </c>
       <c r="AD10" s="26">
         <f t="shared" si="2"/>
-        <v>110085</v>
+        <v>115450</v>
       </c>
       <c r="AE10" s="26">
         <f t="shared" si="2"/>
-        <v>145711</v>
+        <v>139403</v>
       </c>
       <c r="AF10" s="26">
         <f t="shared" si="2"/>
-        <v>132779</v>
+        <v>134505</v>
       </c>
       <c r="AG10" s="26">
         <f t="shared" si="2"/>
-        <v>127243</v>
+        <v>104880</v>
       </c>
       <c r="AH10" s="26">
         <f t="shared" si="2"/>
-        <v>116740</v>
+        <v>121755</v>
       </c>
       <c r="AI10" s="26">
         <f t="shared" si="2"/>
-        <v>122453</v>
+        <v>133154</v>
       </c>
       <c r="AJ10" s="26">
         <f t="shared" si="2"/>
-        <v>147240</v>
+        <v>128855</v>
       </c>
       <c r="AK10" s="26">
         <f t="shared" si="2"/>
-        <v>108572</v>
+        <v>144031</v>
       </c>
       <c r="AL10" s="26">
         <f t="shared" si="2"/>
-        <v>125046</v>
+        <v>123665</v>
       </c>
       <c r="AM10" s="26">
         <f t="shared" si="2"/>
-        <v>147505</v>
+        <v>133617</v>
       </c>
       <c r="AN10" s="26">
         <f t="shared" si="2"/>
-        <v>109259</v>
+        <v>138155</v>
       </c>
       <c r="AO10" s="26">
         <f t="shared" si="2"/>
-        <v>111158</v>
+        <v>124175</v>
       </c>
       <c r="AP10" s="26">
         <f t="shared" si="2"/>
-        <v>130391</v>
+        <v>147187</v>
       </c>
       <c r="AQ10" s="26">
         <f t="shared" si="2"/>
-        <v>147830</v>
+        <v>126847</v>
       </c>
       <c r="AR10" s="26">
         <f t="shared" si="2"/>
-        <v>119927</v>
+        <v>107057</v>
       </c>
       <c r="AS10" s="26">
         <f t="shared" si="2"/>
-        <v>120825</v>
+        <v>145238</v>
       </c>
       <c r="AT10" s="26">
         <f t="shared" si="2"/>
-        <v>100549</v>
+        <v>122971</v>
       </c>
       <c r="AU10" s="26">
         <f t="shared" si="2"/>
-        <v>110894</v>
+        <v>142624</v>
       </c>
       <c r="AV10" s="26">
         <f t="shared" si="2"/>
-        <v>112988</v>
+        <v>108527</v>
       </c>
       <c r="AW10" s="26">
         <f t="shared" si="2"/>
-        <v>122960</v>
+        <v>127734</v>
       </c>
       <c r="AX10" s="26">
         <f t="shared" si="2"/>
-        <v>133038</v>
+        <v>104993</v>
       </c>
       <c r="AY10" s="26">
         <f t="shared" si="2"/>
-        <v>106208</v>
+        <v>102256</v>
       </c>
       <c r="AZ10" s="26">
         <f t="shared" si="2"/>
-        <v>146428</v>
+        <v>101258</v>
       </c>
       <c r="BA10" s="26">
         <f t="shared" si="2"/>
-        <v>100980</v>
+        <v>107740</v>
       </c>
       <c r="BB10" s="26">
         <f t="shared" si="2"/>
-        <v>132365</v>
+        <v>108297</v>
       </c>
       <c r="BC10" s="26">
         <f t="shared" si="2"/>
-        <v>130158</v>
+        <v>105489</v>
       </c>
       <c r="BD10" s="26">
         <f t="shared" si="2"/>
-        <v>144732</v>
+        <v>141458</v>
       </c>
       <c r="BE10" s="26">
         <f t="shared" si="2"/>
-        <v>130794</v>
+        <v>122239</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -1880,211 +1871,211 @@
       </c>
       <c r="F12" s="29">
         <f t="shared" ref="F12:BE12" si="3">IF( $B10="Maximum", F10/F11 , IF( 100%-(F10-F11)/F11 &gt; 0, 100%-(F10-F11)/F11, 0) )</f>
-        <v>1.185408</v>
+        <v>0.950688</v>
       </c>
       <c r="G12" s="29">
         <f t="shared" si="3"/>
-        <v>0.807584</v>
+        <v>0.9476</v>
       </c>
       <c r="H12" s="29">
         <f t="shared" si="3"/>
-        <v>0.803232</v>
+        <v>0.836472</v>
       </c>
       <c r="I12" s="29">
         <f t="shared" si="3"/>
-        <v>1.1798</v>
+        <v>1.021272</v>
       </c>
       <c r="J12" s="29">
         <f t="shared" si="3"/>
-        <v>1.020728</v>
+        <v>0.823192</v>
       </c>
       <c r="K12" s="29">
         <f t="shared" si="3"/>
-        <v>1.036304</v>
+        <v>0.957976</v>
       </c>
       <c r="L12" s="29">
         <f t="shared" si="3"/>
-        <v>0.847808</v>
+        <v>1.149432</v>
       </c>
       <c r="M12" s="29">
         <f t="shared" si="3"/>
-        <v>1.199792</v>
+        <v>1.172696</v>
       </c>
       <c r="N12" s="29">
         <f t="shared" si="3"/>
-        <v>0.958088</v>
+        <v>1.09828</v>
       </c>
       <c r="O12" s="29">
         <f t="shared" si="3"/>
-        <v>0.911752</v>
+        <v>1.15728</v>
       </c>
       <c r="P12" s="29">
         <f t="shared" si="3"/>
-        <v>1.07408</v>
+        <v>1.142344</v>
       </c>
       <c r="Q12" s="29">
         <f t="shared" si="3"/>
-        <v>0.907464</v>
+        <v>1.118528</v>
       </c>
       <c r="R12" s="29">
         <f t="shared" si="3"/>
-        <v>1.112856</v>
+        <v>0.970368</v>
       </c>
       <c r="S12" s="29">
         <f t="shared" si="3"/>
-        <v>0.911528</v>
+        <v>1.069432</v>
       </c>
       <c r="T12" s="29">
         <f t="shared" si="3"/>
-        <v>0.969992</v>
+        <v>0.86436</v>
       </c>
       <c r="U12" s="29">
         <f t="shared" si="3"/>
-        <v>0.97128</v>
+        <v>1.047512</v>
       </c>
       <c r="V12" s="29">
         <f t="shared" si="3"/>
-        <v>1.148424</v>
+        <v>0.877888</v>
       </c>
       <c r="W12" s="29">
         <f t="shared" si="3"/>
-        <v>1.164712</v>
+        <v>1.067504</v>
       </c>
       <c r="X12" s="29">
         <f t="shared" si="3"/>
-        <v>0.926576</v>
+        <v>1.01092</v>
       </c>
       <c r="Y12" s="29">
         <f t="shared" si="3"/>
-        <v>0.99848</v>
+        <v>1.028216</v>
       </c>
       <c r="Z12" s="29">
         <f t="shared" si="3"/>
-        <v>1.128496</v>
+        <v>1.103392</v>
       </c>
       <c r="AA12" s="29">
         <f t="shared" si="3"/>
-        <v>0.924128</v>
+        <v>1.013592</v>
       </c>
       <c r="AB12" s="29">
         <f t="shared" si="3"/>
-        <v>0.958736</v>
+        <v>0.88972</v>
       </c>
       <c r="AC12" s="29">
         <f t="shared" si="3"/>
-        <v>0.801656</v>
+        <v>0.926256</v>
       </c>
       <c r="AD12" s="29">
         <f t="shared" si="3"/>
-        <v>0.88068</v>
+        <v>1.0764</v>
       </c>
       <c r="AE12" s="29">
         <f t="shared" si="3"/>
-        <v>1.165688</v>
+        <v>0.884776</v>
       </c>
       <c r="AF12" s="29">
         <f t="shared" si="3"/>
-        <v>1.062232</v>
+        <v>0.92396</v>
       </c>
       <c r="AG12" s="29">
         <f t="shared" si="3"/>
-        <v>1.017944</v>
+        <v>1.16096</v>
       </c>
       <c r="AH12" s="29">
         <f t="shared" si="3"/>
-        <v>0.93392</v>
+        <v>1.02596</v>
       </c>
       <c r="AI12" s="29">
         <f t="shared" si="3"/>
-        <v>0.979624</v>
+        <v>0.934768</v>
       </c>
       <c r="AJ12" s="29">
         <f t="shared" si="3"/>
-        <v>1.17792</v>
+        <v>0.96916</v>
       </c>
       <c r="AK12" s="29">
         <f t="shared" si="3"/>
-        <v>0.868576</v>
+        <v>0.847752</v>
       </c>
       <c r="AL12" s="29">
         <f t="shared" si="3"/>
-        <v>1.000368</v>
+        <v>1.01068</v>
       </c>
       <c r="AM12" s="29">
         <f t="shared" si="3"/>
-        <v>1.18004</v>
+        <v>0.931064</v>
       </c>
       <c r="AN12" s="29">
         <f t="shared" si="3"/>
-        <v>0.874072</v>
+        <v>0.89476</v>
       </c>
       <c r="AO12" s="29">
         <f t="shared" si="3"/>
-        <v>0.889264</v>
+        <v>1.0066</v>
       </c>
       <c r="AP12" s="29">
         <f t="shared" si="3"/>
-        <v>1.043128</v>
+        <v>0.822504</v>
       </c>
       <c r="AQ12" s="29">
         <f t="shared" si="3"/>
-        <v>1.18264</v>
+        <v>0.985224</v>
       </c>
       <c r="AR12" s="29">
         <f t="shared" si="3"/>
-        <v>0.959416</v>
+        <v>1.143544</v>
       </c>
       <c r="AS12" s="29">
         <f t="shared" si="3"/>
-        <v>0.9666</v>
+        <v>0.838096</v>
       </c>
       <c r="AT12" s="29">
         <f t="shared" si="3"/>
-        <v>0.804392</v>
+        <v>1.016232</v>
       </c>
       <c r="AU12" s="29">
         <f t="shared" si="3"/>
-        <v>0.887152</v>
+        <v>0.859008</v>
       </c>
       <c r="AV12" s="29">
         <f t="shared" si="3"/>
-        <v>0.903904</v>
+        <v>1.131784</v>
       </c>
       <c r="AW12" s="29">
         <f t="shared" si="3"/>
-        <v>0.98368</v>
+        <v>0.978128</v>
       </c>
       <c r="AX12" s="29">
         <f t="shared" si="3"/>
-        <v>1.064304</v>
+        <v>1.160056</v>
       </c>
       <c r="AY12" s="29">
         <f t="shared" si="3"/>
-        <v>0.849664</v>
+        <v>1.181952</v>
       </c>
       <c r="AZ12" s="29">
         <f t="shared" si="3"/>
-        <v>1.171424</v>
+        <v>1.189936</v>
       </c>
       <c r="BA12" s="29">
         <f t="shared" si="3"/>
-        <v>0.80784</v>
+        <v>1.13808</v>
       </c>
       <c r="BB12" s="29">
         <f t="shared" si="3"/>
-        <v>1.05892</v>
+        <v>1.133624</v>
       </c>
       <c r="BC12" s="29">
         <f t="shared" si="3"/>
-        <v>1.041264</v>
+        <v>1.156088</v>
       </c>
       <c r="BD12" s="29">
         <f t="shared" si="3"/>
-        <v>1.157856</v>
+        <v>0.868336</v>
       </c>
       <c r="BE12" s="29">
         <f t="shared" si="3"/>
-        <v>1.046352</v>
+        <v>1.022088</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -2092,11 +2083,11 @@
         <v>18</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C13" s="25">
         <f t="array" ref="C13">IF( B14="Short-Term", AVERAGE(F15:BE15)*B15, INDEX(F15:BE15, 1, COUNTA(F15:BE15))*B15 )</f>
-        <v>0.1796983516</v>
+        <v>0.1897489011</v>
       </c>
       <c r="D13" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B14=""Short-Term"", SPARKLINE(F15:BE15,IF(B13=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F15:BE15, 1, COUNTA(F15:BE15)) ,IF(B13=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -2107,216 +2098,216 @@
       </c>
       <c r="F13" s="26">
         <f t="shared" ref="F13:BE13" si="4">RANDBETWEEN(5000,10000)</f>
-        <v>7582</v>
+        <v>8525</v>
       </c>
       <c r="G13" s="26">
         <f t="shared" si="4"/>
-        <v>7045</v>
+        <v>6857</v>
       </c>
       <c r="H13" s="26">
         <f t="shared" si="4"/>
-        <v>7251</v>
+        <v>9442</v>
       </c>
       <c r="I13" s="26">
         <f t="shared" si="4"/>
-        <v>9382</v>
+        <v>8954</v>
       </c>
       <c r="J13" s="26">
         <f t="shared" si="4"/>
-        <v>7188</v>
+        <v>7146</v>
       </c>
       <c r="K13" s="26">
         <f t="shared" si="4"/>
-        <v>7847</v>
+        <v>8613</v>
       </c>
       <c r="L13" s="26">
         <f t="shared" si="4"/>
-        <v>5944</v>
+        <v>7886</v>
       </c>
       <c r="M13" s="26">
         <f t="shared" si="4"/>
-        <v>8337</v>
+        <v>5699</v>
       </c>
       <c r="N13" s="26">
         <f t="shared" si="4"/>
-        <v>7092</v>
+        <v>5847</v>
       </c>
       <c r="O13" s="26">
         <f t="shared" si="4"/>
-        <v>6282</v>
+        <v>7674</v>
       </c>
       <c r="P13" s="26">
         <f t="shared" si="4"/>
-        <v>8123</v>
+        <v>5361</v>
       </c>
       <c r="Q13" s="26">
         <f t="shared" si="4"/>
-        <v>8920</v>
+        <v>5764</v>
       </c>
       <c r="R13" s="26">
         <f t="shared" si="4"/>
-        <v>6410</v>
+        <v>8999</v>
       </c>
       <c r="S13" s="26">
         <f t="shared" si="4"/>
-        <v>7477</v>
+        <v>8556</v>
       </c>
       <c r="T13" s="26">
         <f t="shared" si="4"/>
-        <v>8102</v>
+        <v>7191</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="4"/>
-        <v>6280</v>
+        <v>8781</v>
       </c>
       <c r="V13" s="26">
         <f t="shared" si="4"/>
-        <v>5255</v>
+        <v>8266</v>
       </c>
       <c r="W13" s="26">
         <f t="shared" si="4"/>
-        <v>9707</v>
+        <v>5808</v>
       </c>
       <c r="X13" s="26">
         <f t="shared" si="4"/>
-        <v>9107</v>
+        <v>8331</v>
       </c>
       <c r="Y13" s="26">
         <f t="shared" si="4"/>
-        <v>9182</v>
+        <v>9034</v>
       </c>
       <c r="Z13" s="26">
         <f t="shared" si="4"/>
-        <v>8549</v>
+        <v>9024</v>
       </c>
       <c r="AA13" s="26">
         <f t="shared" si="4"/>
-        <v>7074</v>
+        <v>6546</v>
       </c>
       <c r="AB13" s="26">
         <f t="shared" si="4"/>
-        <v>8512</v>
+        <v>5691</v>
       </c>
       <c r="AC13" s="26">
         <f t="shared" si="4"/>
-        <v>9502</v>
+        <v>5190</v>
       </c>
       <c r="AD13" s="26">
         <f t="shared" si="4"/>
-        <v>5321</v>
+        <v>6204</v>
       </c>
       <c r="AE13" s="26">
         <f t="shared" si="4"/>
-        <v>5045</v>
+        <v>5559</v>
       </c>
       <c r="AF13" s="26">
         <f t="shared" si="4"/>
-        <v>5758</v>
+        <v>8280</v>
       </c>
       <c r="AG13" s="26">
         <f t="shared" si="4"/>
-        <v>9119</v>
+        <v>9819</v>
       </c>
       <c r="AH13" s="26">
         <f t="shared" si="4"/>
-        <v>7785</v>
+        <v>9291</v>
       </c>
       <c r="AI13" s="26">
         <f t="shared" si="4"/>
-        <v>6836</v>
+        <v>7398</v>
       </c>
       <c r="AJ13" s="26">
         <f t="shared" si="4"/>
-        <v>8690</v>
+        <v>7990</v>
       </c>
       <c r="AK13" s="26">
         <f t="shared" si="4"/>
-        <v>9356</v>
+        <v>9778</v>
       </c>
       <c r="AL13" s="26">
         <f t="shared" si="4"/>
-        <v>7248</v>
+        <v>7189</v>
       </c>
       <c r="AM13" s="26">
         <f t="shared" si="4"/>
-        <v>5746</v>
+        <v>9497</v>
       </c>
       <c r="AN13" s="26">
         <f t="shared" si="4"/>
-        <v>9711</v>
+        <v>5019</v>
       </c>
       <c r="AO13" s="26">
         <f t="shared" si="4"/>
-        <v>8901</v>
+        <v>6433</v>
       </c>
       <c r="AP13" s="26">
         <f t="shared" si="4"/>
-        <v>8718</v>
+        <v>6130</v>
       </c>
       <c r="AQ13" s="26">
         <f t="shared" si="4"/>
-        <v>9078</v>
+        <v>7697</v>
       </c>
       <c r="AR13" s="26">
         <f t="shared" si="4"/>
-        <v>8313</v>
+        <v>6867</v>
       </c>
       <c r="AS13" s="26">
         <f t="shared" si="4"/>
-        <v>7543</v>
+        <v>7644</v>
       </c>
       <c r="AT13" s="26">
         <f t="shared" si="4"/>
-        <v>7866</v>
+        <v>7607</v>
       </c>
       <c r="AU13" s="26">
         <f t="shared" si="4"/>
-        <v>7920</v>
+        <v>5507</v>
       </c>
       <c r="AV13" s="26">
         <f t="shared" si="4"/>
-        <v>6277</v>
+        <v>8780</v>
       </c>
       <c r="AW13" s="26">
         <f t="shared" si="4"/>
-        <v>5362</v>
+        <v>6649</v>
       </c>
       <c r="AX13" s="26">
         <f t="shared" si="4"/>
-        <v>7871</v>
+        <v>8552</v>
       </c>
       <c r="AY13" s="26">
         <f t="shared" si="4"/>
-        <v>9188</v>
+        <v>6058</v>
       </c>
       <c r="AZ13" s="26">
         <f t="shared" si="4"/>
-        <v>6054</v>
+        <v>6343</v>
       </c>
       <c r="BA13" s="26">
         <f t="shared" si="4"/>
-        <v>9986</v>
+        <v>6306</v>
       </c>
       <c r="BB13" s="26">
         <f t="shared" si="4"/>
-        <v>9565</v>
+        <v>7665</v>
       </c>
       <c r="BC13" s="26">
         <f t="shared" si="4"/>
-        <v>6512</v>
+        <v>5975</v>
       </c>
       <c r="BD13" s="26">
         <f t="shared" si="4"/>
-        <v>6632</v>
+        <v>7631</v>
       </c>
       <c r="BE13" s="26">
         <f t="shared" si="4"/>
-        <v>8398</v>
+        <v>5604</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>22</v>
@@ -2490,211 +2481,211 @@
       </c>
       <c r="F15" s="29">
         <f t="shared" ref="F15:BE15" si="5">IF( $B13="Maximum", F13/F14 , IF( 100%-(F13-F14)/F14 &gt; 0, 100%-(F13-F14)/F14, 0) )</f>
-        <v>0.9168571429</v>
+        <v>0.7821428571</v>
       </c>
       <c r="G15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9935714286</v>
+        <v>1.020428571</v>
       </c>
       <c r="H15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9641428571</v>
+        <v>0.6511428571</v>
       </c>
       <c r="I15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6597142857</v>
+        <v>0.7208571429</v>
       </c>
       <c r="J15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9731428571</v>
+        <v>0.9791428571</v>
       </c>
       <c r="K15" s="29">
         <f t="shared" si="5"/>
-        <v>0.879</v>
+        <v>0.7695714286</v>
       </c>
       <c r="L15" s="29">
         <f t="shared" si="5"/>
-        <v>1.150857143</v>
+        <v>0.8734285714</v>
       </c>
       <c r="M15" s="29">
         <f t="shared" si="5"/>
-        <v>0.809</v>
+        <v>1.185857143</v>
       </c>
       <c r="N15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9868571429</v>
+        <v>1.164714286</v>
       </c>
       <c r="O15" s="29">
         <f t="shared" si="5"/>
-        <v>1.102571429</v>
+        <v>0.9037142857</v>
       </c>
       <c r="P15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8395714286</v>
+        <v>1.234142857</v>
       </c>
       <c r="Q15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7257142857</v>
+        <v>1.176571429</v>
       </c>
       <c r="R15" s="29">
         <f t="shared" si="5"/>
-        <v>1.084285714</v>
+        <v>0.7144285714</v>
       </c>
       <c r="S15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9318571429</v>
+        <v>0.7777142857</v>
       </c>
       <c r="T15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8425714286</v>
+        <v>0.9727142857</v>
       </c>
       <c r="U15" s="29">
         <f t="shared" si="5"/>
-        <v>1.102857143</v>
+        <v>0.7455714286</v>
       </c>
       <c r="V15" s="29">
         <f t="shared" si="5"/>
-        <v>1.249285714</v>
+        <v>0.8191428571</v>
       </c>
       <c r="W15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6132857143</v>
+        <v>1.170285714</v>
       </c>
       <c r="X15" s="29">
         <f t="shared" si="5"/>
-        <v>0.699</v>
+        <v>0.8098571429</v>
       </c>
       <c r="Y15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6882857143</v>
+        <v>0.7094285714</v>
       </c>
       <c r="Z15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7787142857</v>
+        <v>0.7108571429</v>
       </c>
       <c r="AA15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9894285714</v>
+        <v>1.064857143</v>
       </c>
       <c r="AB15" s="29">
         <f t="shared" si="5"/>
-        <v>0.784</v>
+        <v>1.187</v>
       </c>
       <c r="AC15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6425714286</v>
+        <v>1.258571429</v>
       </c>
       <c r="AD15" s="29">
         <f t="shared" si="5"/>
-        <v>1.239857143</v>
+        <v>1.113714286</v>
       </c>
       <c r="AE15" s="29">
         <f t="shared" si="5"/>
-        <v>1.279285714</v>
+        <v>1.205857143</v>
       </c>
       <c r="AF15" s="29">
         <f t="shared" si="5"/>
-        <v>1.177428571</v>
+        <v>0.8171428571</v>
       </c>
       <c r="AG15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6972857143</v>
+        <v>0.5972857143</v>
       </c>
       <c r="AH15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8878571429</v>
+        <v>0.6727142857</v>
       </c>
       <c r="AI15" s="29">
         <f t="shared" si="5"/>
-        <v>1.023428571</v>
+        <v>0.9431428571</v>
       </c>
       <c r="AJ15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7585714286</v>
+        <v>0.8585714286</v>
       </c>
       <c r="AK15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6634285714</v>
+        <v>0.6031428571</v>
       </c>
       <c r="AL15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9645714286</v>
+        <v>0.973</v>
       </c>
       <c r="AM15" s="29">
         <f t="shared" si="5"/>
-        <v>1.179142857</v>
+        <v>0.6432857143</v>
       </c>
       <c r="AN15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6127142857</v>
+        <v>1.283</v>
       </c>
       <c r="AO15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7284285714</v>
+        <v>1.081</v>
       </c>
       <c r="AP15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7545714286</v>
+        <v>1.124285714</v>
       </c>
       <c r="AQ15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7031428571</v>
+        <v>0.9004285714</v>
       </c>
       <c r="AR15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8124285714</v>
+        <v>1.019</v>
       </c>
       <c r="AS15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9224285714</v>
+        <v>0.908</v>
       </c>
       <c r="AT15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8762857143</v>
+        <v>0.9132857143</v>
       </c>
       <c r="AU15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8685714286</v>
+        <v>1.213285714</v>
       </c>
       <c r="AV15" s="29">
         <f t="shared" si="5"/>
-        <v>1.103285714</v>
+        <v>0.7457142857</v>
       </c>
       <c r="AW15" s="29">
         <f t="shared" si="5"/>
-        <v>1.234</v>
+        <v>1.050142857</v>
       </c>
       <c r="AX15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8755714286</v>
+        <v>0.7782857143</v>
       </c>
       <c r="AY15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6874285714</v>
+        <v>1.134571429</v>
       </c>
       <c r="AZ15" s="29">
         <f t="shared" si="5"/>
-        <v>1.135142857</v>
+        <v>1.093857143</v>
       </c>
       <c r="BA15" s="29">
         <f t="shared" si="5"/>
-        <v>0.5734285714</v>
+        <v>1.099142857</v>
       </c>
       <c r="BB15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6335714286</v>
+        <v>0.905</v>
       </c>
       <c r="BC15" s="29">
         <f t="shared" si="5"/>
-        <v>1.069714286</v>
+        <v>1.146428571</v>
       </c>
       <c r="BD15" s="29">
         <f t="shared" si="5"/>
-        <v>1.052571429</v>
+        <v>0.9098571429</v>
       </c>
       <c r="BE15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8002857143</v>
+        <v>1.199428571</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -2702,7 +2693,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C16" s="25">
         <f t="array" ref="C16">IF( B17="Short-Term", AVERAGE(F18:BE18)*B18, INDEX(F18:BE18, 1, COUNTA(F18:BE18))*B18 )</f>
@@ -3260,7 +3251,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C19" s="25">
         <f t="array" ref="C19">IF( B20="Short-Term", AVERAGE(F21:BE21)*B21, INDEX(F21:BE21, 1, COUNTA(F21:BE21))*B21 )</f>
@@ -3896,7 +3887,7 @@
         <v>30</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C25" s="25">
         <f t="array" ref="C25">IF( B26="Short-Term", AVERAGE(F27:BE27)*B27, INDEX(F27:BE27, 1, COUNTA(F27:BE27))*B27 )</f>
@@ -4470,7 +4461,7 @@
       <c r="B30" s="19"/>
       <c r="C30" s="20">
         <f>SUMIFS(C31:C1013,A31:A1013,A31)</f>
-        <v>0.7252884615</v>
+        <v>0.7341730769</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
@@ -4532,11 +4523,11 @@
         <v>32</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C31" s="25">
         <f t="array" ref="C31">IF( B32="Short-Term", AVERAGE(F33:BE33)*B33, INDEX(F33:BE33, 1, COUNTA(F33:BE33))*B33 )</f>
-        <v>0.3661538462</v>
+        <v>0.3755769231</v>
       </c>
       <c r="D31" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B32=""Short-Term"", SPARKLINE(F33:BE33,IF(B31=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F33:BE33, 1, COUNTA(F33:BE33)) ,IF(B31=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -4547,47 +4538,47 @@
       </c>
       <c r="F31" s="26">
         <f t="shared" ref="F31:BE31" si="9">RANDBETWEEN(1,50)</f>
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="G31" s="26">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H31" s="26">
         <f t="shared" si="9"/>
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="I31" s="26">
         <f t="shared" si="9"/>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J31" s="26">
         <f t="shared" si="9"/>
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="K31" s="26">
         <f t="shared" si="9"/>
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="L31" s="26">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="M31" s="26">
         <f t="shared" si="9"/>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N31" s="26">
         <f t="shared" si="9"/>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O31" s="26">
         <f t="shared" si="9"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="P31" s="26">
         <f t="shared" si="9"/>
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="Q31" s="26">
         <f t="shared" si="9"/>
@@ -4595,43 +4586,43 @@
       </c>
       <c r="R31" s="26">
         <f t="shared" si="9"/>
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="S31" s="26">
         <f t="shared" si="9"/>
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="T31" s="26">
         <f t="shared" si="9"/>
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="U31" s="26">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="V31" s="26">
         <f t="shared" si="9"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="W31" s="26">
         <f t="shared" si="9"/>
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="X31" s="26">
         <f t="shared" si="9"/>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="Y31" s="26">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="Z31" s="26">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="AA31" s="26">
         <f t="shared" si="9"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AB31" s="26">
         <f t="shared" si="9"/>
@@ -4643,7 +4634,7 @@
       </c>
       <c r="AD31" s="26">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="AE31" s="26">
         <f t="shared" si="9"/>
@@ -4651,107 +4642,107 @@
       </c>
       <c r="AF31" s="26">
         <f t="shared" si="9"/>
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="AG31" s="26">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="AH31" s="26">
         <f t="shared" si="9"/>
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="AI31" s="26">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="AJ31" s="26">
         <f t="shared" si="9"/>
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="AK31" s="26">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="AL31" s="26">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="AM31" s="26">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="AN31" s="26">
         <f t="shared" si="9"/>
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="AO31" s="26">
         <f t="shared" si="9"/>
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="AP31" s="26">
         <f t="shared" si="9"/>
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AQ31" s="26">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="AR31" s="26">
         <f t="shared" si="9"/>
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="AS31" s="26">
         <f t="shared" si="9"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="AT31" s="26">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AU31" s="26">
         <f t="shared" si="9"/>
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="AV31" s="26">
         <f t="shared" si="9"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AW31" s="26">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="AX31" s="26">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="AY31" s="26">
         <f t="shared" si="9"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AZ31" s="26">
         <f t="shared" si="9"/>
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="BA31" s="26">
         <f t="shared" si="9"/>
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="BB31" s="26">
         <f t="shared" si="9"/>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="BC31" s="26">
         <f t="shared" si="9"/>
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="BD31" s="26">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="BE31" s="26">
         <f t="shared" si="9"/>
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -4930,47 +4921,47 @@
       </c>
       <c r="F33" s="29">
         <f t="shared" ref="F33:BE33" si="10">IF( $B31="Maximum", F31/F32 , IF( 100%-(F31-F32)/F32 &gt; 0, 100%-(F31-F32)/F32, 0) )</f>
-        <v>0.24</v>
+        <v>0.96</v>
       </c>
       <c r="G33" s="29">
         <f t="shared" si="10"/>
-        <v>0.06</v>
+        <v>0.68</v>
       </c>
       <c r="H33" s="29">
         <f t="shared" si="10"/>
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="I33" s="29">
         <f t="shared" si="10"/>
-        <v>0.88</v>
+        <v>0.82</v>
       </c>
       <c r="J33" s="29">
         <f t="shared" si="10"/>
-        <v>0.82</v>
+        <v>0.96</v>
       </c>
       <c r="K33" s="29">
         <f t="shared" si="10"/>
-        <v>0.74</v>
+        <v>0.52</v>
       </c>
       <c r="L33" s="29">
         <f t="shared" si="10"/>
-        <v>0.04</v>
+        <v>0.96</v>
       </c>
       <c r="M33" s="29">
         <f t="shared" si="10"/>
-        <v>0.56</v>
+        <v>0.64</v>
       </c>
       <c r="N33" s="29">
         <f t="shared" si="10"/>
-        <v>0.44</v>
+        <v>0.56</v>
       </c>
       <c r="O33" s="29">
         <f t="shared" si="10"/>
-        <v>0.48</v>
+        <v>0.4</v>
       </c>
       <c r="P33" s="29">
         <f t="shared" si="10"/>
-        <v>0.56</v>
+        <v>0.78</v>
       </c>
       <c r="Q33" s="29">
         <f t="shared" si="10"/>
@@ -4978,43 +4969,43 @@
       </c>
       <c r="R33" s="29">
         <f t="shared" si="10"/>
-        <v>0.74</v>
+        <v>0.3</v>
       </c>
       <c r="S33" s="29">
         <f t="shared" si="10"/>
-        <v>0.64</v>
+        <v>0.26</v>
       </c>
       <c r="T33" s="29">
         <f t="shared" si="10"/>
-        <v>0.72</v>
+        <v>1</v>
       </c>
       <c r="U33" s="29">
         <f t="shared" si="10"/>
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="V33" s="29">
         <f t="shared" si="10"/>
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
       <c r="W33" s="29">
         <f t="shared" si="10"/>
-        <v>0.76</v>
+        <v>0.9</v>
       </c>
       <c r="X33" s="29">
         <f t="shared" si="10"/>
-        <v>0.42</v>
+        <v>0.34</v>
       </c>
       <c r="Y33" s="29">
         <f t="shared" si="10"/>
-        <v>0.16</v>
+        <v>0.66</v>
       </c>
       <c r="Z33" s="29">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.32</v>
       </c>
       <c r="AA33" s="29">
         <f t="shared" si="10"/>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="AB33" s="29">
         <f t="shared" si="10"/>
@@ -5026,7 +5017,7 @@
       </c>
       <c r="AD33" s="29">
         <f t="shared" si="10"/>
-        <v>0.02</v>
+        <v>0.52</v>
       </c>
       <c r="AE33" s="29">
         <f t="shared" si="10"/>
@@ -5034,107 +5025,107 @@
       </c>
       <c r="AF33" s="29">
         <f t="shared" si="10"/>
-        <v>0.92</v>
+        <v>0.38</v>
       </c>
       <c r="AG33" s="29">
         <f t="shared" si="10"/>
-        <v>0.24</v>
+        <v>0.68</v>
       </c>
       <c r="AH33" s="29">
         <f t="shared" si="10"/>
-        <v>0.8</v>
+        <v>0.28</v>
       </c>
       <c r="AI33" s="29">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.56</v>
       </c>
       <c r="AJ33" s="29">
         <f t="shared" si="10"/>
-        <v>0.86</v>
+        <v>0.6</v>
       </c>
       <c r="AK33" s="29">
         <f t="shared" si="10"/>
-        <v>0.08</v>
+        <v>0.9</v>
       </c>
       <c r="AL33" s="29">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="AM33" s="29">
         <f t="shared" si="10"/>
-        <v>0.16</v>
+        <v>0.7</v>
       </c>
       <c r="AN33" s="29">
         <f t="shared" si="10"/>
-        <v>0.88</v>
+        <v>0.22</v>
       </c>
       <c r="AO33" s="29">
         <f t="shared" si="10"/>
-        <v>0.98</v>
+        <v>0.46</v>
       </c>
       <c r="AP33" s="29">
         <f t="shared" si="10"/>
-        <v>0.96</v>
+        <v>0.86</v>
       </c>
       <c r="AQ33" s="29">
         <f t="shared" si="10"/>
-        <v>0.14</v>
+        <v>0.46</v>
       </c>
       <c r="AR33" s="29">
         <f t="shared" si="10"/>
-        <v>0.6</v>
+        <v>0.32</v>
       </c>
       <c r="AS33" s="29">
         <f t="shared" si="10"/>
-        <v>0.22</v>
+        <v>0.04</v>
       </c>
       <c r="AT33" s="29">
         <f t="shared" si="10"/>
-        <v>0.12</v>
+        <v>0.3</v>
       </c>
       <c r="AU33" s="29">
         <f t="shared" si="10"/>
-        <v>0.62</v>
+        <v>0.08</v>
       </c>
       <c r="AV33" s="29">
         <f t="shared" si="10"/>
-        <v>0.64</v>
+        <v>0.6</v>
       </c>
       <c r="AW33" s="29">
         <f t="shared" si="10"/>
-        <v>0.02</v>
+        <v>0.24</v>
       </c>
       <c r="AX33" s="29">
         <f t="shared" si="10"/>
-        <v>0.02</v>
+        <v>0.28</v>
       </c>
       <c r="AY33" s="29">
         <f t="shared" si="10"/>
-        <v>0.58</v>
+        <v>0.54</v>
       </c>
       <c r="AZ33" s="29">
         <f t="shared" si="10"/>
-        <v>0.64</v>
+        <v>0.24</v>
       </c>
       <c r="BA33" s="29">
         <f t="shared" si="10"/>
-        <v>0.42</v>
+        <v>0.7</v>
       </c>
       <c r="BB33" s="29">
         <f t="shared" si="10"/>
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="BC33" s="29">
         <f t="shared" si="10"/>
-        <v>0.78</v>
+        <v>0.56</v>
       </c>
       <c r="BD33" s="29">
         <f t="shared" si="10"/>
-        <v>0.08</v>
+        <v>0.82</v>
       </c>
       <c r="BE33" s="29">
         <f t="shared" si="10"/>
-        <v>0.34</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -5142,11 +5133,11 @@
         <v>32</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C34" s="25">
         <f t="array" ref="C34">IF( B35="Short-Term", AVERAGE(F36:BE36)*B36, INDEX(F36:BE36, 1, COUNTA(F36:BE36))*B36 )</f>
-        <v>0.02798076923</v>
+        <v>0.02744230769</v>
       </c>
       <c r="D34" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B35=""Short-Term"", SPARKLINE(F36:BE36,IF(B34=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F36:BE36, 1, COUNTA(F36:BE36)) ,IF(B34=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -5157,95 +5148,95 @@
       </c>
       <c r="F34" s="26">
         <f t="shared" ref="F34:BE34" si="11">RANDBETWEEN(1,50)</f>
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="G34" s="26">
         <f t="shared" si="11"/>
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="H34" s="26">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="I34" s="26">
         <f t="shared" si="11"/>
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="J34" s="26">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="K34" s="26">
         <f t="shared" si="11"/>
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="L34" s="26">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="M34" s="26">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="N34" s="26">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="O34" s="26">
         <f t="shared" si="11"/>
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="P34" s="26">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="Q34" s="26">
         <f t="shared" si="11"/>
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="R34" s="26">
         <f t="shared" si="11"/>
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="S34" s="26">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="T34" s="26">
         <f t="shared" si="11"/>
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="U34" s="26">
         <f t="shared" si="11"/>
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="V34" s="26">
         <f t="shared" si="11"/>
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="W34" s="26">
         <f t="shared" si="11"/>
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="X34" s="26">
         <f t="shared" si="11"/>
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="Y34" s="26">
         <f t="shared" si="11"/>
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="Z34" s="26">
         <f t="shared" si="11"/>
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="AA34" s="26">
         <f t="shared" si="11"/>
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AB34" s="26">
         <f t="shared" si="11"/>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AC34" s="26">
         <f t="shared" si="11"/>
@@ -5253,115 +5244,115 @@
       </c>
       <c r="AD34" s="26">
         <f t="shared" si="11"/>
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="AE34" s="26">
         <f t="shared" si="11"/>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AF34" s="26">
         <f t="shared" si="11"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AG34" s="26">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AH34" s="26">
         <f t="shared" si="11"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI34" s="26">
         <f t="shared" si="11"/>
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="AJ34" s="26">
         <f t="shared" si="11"/>
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="AK34" s="26">
         <f t="shared" si="11"/>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AL34" s="26">
         <f t="shared" si="11"/>
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AM34" s="26">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="AN34" s="26">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="AO34" s="26">
         <f t="shared" si="11"/>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="AP34" s="26">
         <f t="shared" si="11"/>
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="AQ34" s="26">
         <f t="shared" si="11"/>
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="AR34" s="26">
         <f t="shared" si="11"/>
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="AS34" s="26">
         <f t="shared" si="11"/>
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="AT34" s="26">
         <f t="shared" si="11"/>
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="AU34" s="26">
         <f t="shared" si="11"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AV34" s="26">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="AW34" s="26">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="AX34" s="26">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="AY34" s="26">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="AZ34" s="26">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="BA34" s="26">
         <f t="shared" si="11"/>
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="BB34" s="26">
         <f t="shared" si="11"/>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="BC34" s="26">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="BD34" s="26">
         <f t="shared" si="11"/>
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="BE34" s="26">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -5540,95 +5531,95 @@
       </c>
       <c r="F36" s="29">
         <f t="shared" ref="F36:BE36" si="12">IF( $B34="Maximum", F34/F35 , IF( 100%-(F34-F35)/F35 &gt; 0, 100%-(F34-F35)/F35, 0) )</f>
-        <v>0.16</v>
+        <v>0.48</v>
       </c>
       <c r="G36" s="29">
         <f t="shared" si="12"/>
-        <v>0.29</v>
+        <v>0.1</v>
       </c>
       <c r="H36" s="29">
         <f t="shared" si="12"/>
-        <v>0.06</v>
+        <v>0.3</v>
       </c>
       <c r="I36" s="29">
         <f t="shared" si="12"/>
-        <v>0.16</v>
+        <v>0.3</v>
       </c>
       <c r="J36" s="29">
         <f t="shared" si="12"/>
-        <v>0.13</v>
+        <v>0.04</v>
       </c>
       <c r="K36" s="29">
         <f t="shared" si="12"/>
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
       <c r="L36" s="29">
         <f t="shared" si="12"/>
-        <v>0.03</v>
+        <v>0.33</v>
       </c>
       <c r="M36" s="29">
         <f t="shared" si="12"/>
-        <v>0.13</v>
+        <v>0.36</v>
       </c>
       <c r="N36" s="29">
         <f t="shared" si="12"/>
-        <v>0.08</v>
+        <v>0.35</v>
       </c>
       <c r="O36" s="29">
         <f t="shared" si="12"/>
-        <v>0.44</v>
+        <v>0.13</v>
       </c>
       <c r="P36" s="29">
         <f t="shared" si="12"/>
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="Q36" s="29">
         <f t="shared" si="12"/>
-        <v>0.47</v>
+        <v>0.27</v>
       </c>
       <c r="R36" s="29">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="S36" s="29">
         <f t="shared" si="12"/>
-        <v>0.13</v>
+        <v>0.2</v>
       </c>
       <c r="T36" s="29">
         <f t="shared" si="12"/>
-        <v>0.23</v>
+        <v>0.44</v>
       </c>
       <c r="U36" s="29">
         <f t="shared" si="12"/>
-        <v>0.29</v>
+        <v>0.5</v>
       </c>
       <c r="V36" s="29">
         <f t="shared" si="12"/>
-        <v>0.24</v>
+        <v>0.11</v>
       </c>
       <c r="W36" s="29">
         <f t="shared" si="12"/>
-        <v>0.35</v>
+        <v>0.42</v>
       </c>
       <c r="X36" s="29">
         <f t="shared" si="12"/>
-        <v>0.43</v>
+        <v>0.18</v>
       </c>
       <c r="Y36" s="29">
         <f t="shared" si="12"/>
-        <v>0.48</v>
+        <v>0.15</v>
       </c>
       <c r="Z36" s="29">
         <f t="shared" si="12"/>
-        <v>0.38</v>
+        <v>0.46</v>
       </c>
       <c r="AA36" s="29">
         <f t="shared" si="12"/>
-        <v>0.23</v>
+        <v>0.17</v>
       </c>
       <c r="AB36" s="29">
         <f t="shared" si="12"/>
-        <v>0.37</v>
+        <v>0.35</v>
       </c>
       <c r="AC36" s="29">
         <f t="shared" si="12"/>
@@ -5636,115 +5627,115 @@
       </c>
       <c r="AD36" s="29">
         <f t="shared" si="12"/>
-        <v>0.22</v>
+        <v>0.29</v>
       </c>
       <c r="AE36" s="29">
         <f t="shared" si="12"/>
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="AF36" s="29">
         <f t="shared" si="12"/>
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="AG36" s="29">
         <f t="shared" si="12"/>
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="AH36" s="29">
         <f t="shared" si="12"/>
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="AI36" s="29">
         <f t="shared" si="12"/>
-        <v>0.37</v>
+        <v>0.16</v>
       </c>
       <c r="AJ36" s="29">
         <f t="shared" si="12"/>
-        <v>0.42</v>
+        <v>0.27</v>
       </c>
       <c r="AK36" s="29">
         <f t="shared" si="12"/>
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="AL36" s="29">
         <f t="shared" si="12"/>
-        <v>0.37</v>
+        <v>0.31</v>
       </c>
       <c r="AM36" s="29">
         <f t="shared" si="12"/>
-        <v>0.06</v>
+        <v>0.37</v>
       </c>
       <c r="AN36" s="29">
         <f t="shared" si="12"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AO36" s="29">
         <f t="shared" si="12"/>
-        <v>0.19</v>
+        <v>0.05</v>
       </c>
       <c r="AP36" s="29">
         <f t="shared" si="12"/>
-        <v>0.38</v>
+        <v>0.22</v>
       </c>
       <c r="AQ36" s="29">
         <f t="shared" si="12"/>
-        <v>0.23</v>
+        <v>0.03</v>
       </c>
       <c r="AR36" s="29">
         <f t="shared" si="12"/>
-        <v>0.45</v>
+        <v>0.04</v>
       </c>
       <c r="AS36" s="29">
         <f t="shared" si="12"/>
-        <v>0.35</v>
+        <v>0.48</v>
       </c>
       <c r="AT36" s="29">
         <f t="shared" si="12"/>
-        <v>0.39</v>
+        <v>0.45</v>
       </c>
       <c r="AU36" s="29">
         <f t="shared" si="12"/>
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="AV36" s="29">
         <f t="shared" si="12"/>
-        <v>0.4</v>
+        <v>0.31</v>
       </c>
       <c r="AW36" s="29">
         <f t="shared" si="12"/>
-        <v>0.11</v>
+        <v>0.43</v>
       </c>
       <c r="AX36" s="29">
         <f t="shared" si="12"/>
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="AY36" s="29">
         <f t="shared" si="12"/>
-        <v>0.12</v>
+        <v>0.04</v>
       </c>
       <c r="AZ36" s="29">
         <f t="shared" si="12"/>
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="BA36" s="29">
         <f t="shared" si="12"/>
-        <v>0.27</v>
+        <v>0.05</v>
       </c>
       <c r="BB36" s="29">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.08</v>
       </c>
       <c r="BC36" s="29">
         <f t="shared" si="12"/>
-        <v>0.13</v>
+        <v>0.03</v>
       </c>
       <c r="BD36" s="29">
         <f t="shared" si="12"/>
-        <v>0.35</v>
+        <v>0.19</v>
       </c>
       <c r="BE36" s="29">
         <f t="shared" si="12"/>
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -5752,7 +5743,7 @@
         <v>32</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C37" s="25">
         <f t="array" ref="C37">IF( B38="Short-Term", AVERAGE(F39:BE39)*B39, INDEX(F39:BE39, 1, COUNTA(F39:BE39))*B39 )</f>
@@ -11272,23 +11263,18 @@
     <mergeCell ref="AB6:AE6"/>
     <mergeCell ref="AF6:AI6"/>
   </mergeCells>
-  <conditionalFormatting sqref="F13:BE13 F16:BE16 F19:BE19 F37:BE37">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
-      <formula>F14</formula>
+  <conditionalFormatting sqref="F10:BE10 F13:BE13 F16:BE16 F19:BE19 F25:BE25 F31:BE31 F34:BE34 F37:BE37">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND($B10="Maximum",F10&gt;=F11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:BE10 F13:BE13 F16:BE16 F19:BE19 F25:BE25 F31:BE31 F34:BE34 F37:BE37">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>AND($B10="Maximum",F10&gt;=F11)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10:BE10 F13:BE13 F16:BE16 F19:BE19 F25:BE25 F31:BE31 F34:BE34 F37:BE37">
-    <cfRule type="expression" dxfId="0" priority="3">
       <formula>AND($B10="Minimum",50%&gt;F12)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:BE10 F13:BE13 F16:BE16 F19:BE19 F25:BE25 F31:BE31 F34:BE34 F37:BE37">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(F10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11336,423 +11322,423 @@
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4">
-        <f t="shared" ref="F1:BE1" si="1">AVERAGEIFS(F9:F987,$E9:$E987,"% Target")</f>
-        <v>0.65</v>
+        <f t="shared" ref="F1:BE1" si="1">AVERAGEIFS(F9:F984,$E9:$E984,"% Target")</f>
+        <v>0.8333333333</v>
       </c>
       <c r="G1" s="4">
         <f t="shared" si="1"/>
-        <v>0.63</v>
+        <v>0.8033333333</v>
       </c>
       <c r="H1" s="4">
         <f t="shared" si="1"/>
-        <v>0.61</v>
+        <v>0.7733333333</v>
       </c>
       <c r="I1" s="4">
         <f t="shared" si="1"/>
-        <v>0.44</v>
+        <v>0.5433333333</v>
       </c>
       <c r="J1" s="4">
         <f t="shared" si="1"/>
-        <v>0.42</v>
+        <v>0.5133333333</v>
       </c>
       <c r="K1" s="4">
         <f t="shared" si="1"/>
-        <v>0.525</v>
+        <v>0.65</v>
       </c>
       <c r="L1" s="4">
         <f t="shared" si="1"/>
-        <v>0.68</v>
+        <v>0.8533333333</v>
       </c>
       <c r="M1" s="4">
         <f t="shared" si="1"/>
-        <v>0.66</v>
+        <v>0.8233333333</v>
       </c>
       <c r="N1" s="4">
         <f t="shared" si="1"/>
-        <v>0.64</v>
+        <v>0.7933333333</v>
       </c>
       <c r="O1" s="4">
         <f t="shared" si="1"/>
-        <v>0.47</v>
+        <v>0.5633333333</v>
       </c>
       <c r="P1" s="4">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5333333333</v>
       </c>
       <c r="Q1" s="4">
         <f t="shared" si="1"/>
-        <v>0.555</v>
+        <v>0.67</v>
       </c>
       <c r="R1" s="4">
         <f t="shared" si="1"/>
-        <v>0.71</v>
+        <v>0.8733333333</v>
       </c>
       <c r="S1" s="4">
         <f t="shared" si="1"/>
-        <v>0.69</v>
+        <v>0.8433333333</v>
       </c>
       <c r="T1" s="4">
         <f t="shared" si="1"/>
-        <v>0.67</v>
+        <v>0.8133333333</v>
       </c>
       <c r="U1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.5833333333</v>
       </c>
       <c r="V1" s="4">
         <f t="shared" si="1"/>
-        <v>0.48</v>
+        <v>0.5533333333</v>
       </c>
       <c r="W1" s="4">
         <f t="shared" si="1"/>
-        <v>0.585</v>
+        <v>0.69</v>
       </c>
       <c r="X1" s="4">
         <f t="shared" si="1"/>
-        <v>0.74</v>
+        <v>0.8933333333</v>
       </c>
       <c r="Y1" s="4">
         <f t="shared" si="1"/>
-        <v>0.72</v>
+        <v>0.8633333333</v>
       </c>
       <c r="Z1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>0.8333333333</v>
       </c>
       <c r="AA1" s="4">
         <f t="shared" si="1"/>
-        <v>0.53</v>
+        <v>0.6033333333</v>
       </c>
       <c r="AB1" s="4">
         <f t="shared" si="1"/>
-        <v>0.51</v>
+        <v>0.5733333333</v>
       </c>
       <c r="AC1" s="4">
         <f t="shared" si="1"/>
-        <v>0.615</v>
+        <v>0.71</v>
       </c>
       <c r="AD1" s="4">
         <f t="shared" si="1"/>
-        <v>0.77</v>
+        <v>0.9133333333</v>
       </c>
       <c r="AE1" s="4">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.8833333333</v>
       </c>
       <c r="AF1" s="4">
         <f t="shared" si="1"/>
-        <v>0.73</v>
+        <v>0.8533333333</v>
       </c>
       <c r="AG1" s="4">
         <f t="shared" si="1"/>
-        <v>0.56</v>
+        <v>0.6233333333</v>
       </c>
       <c r="AH1" s="4">
         <f t="shared" si="1"/>
-        <v>0.54</v>
+        <v>0.5933333333</v>
       </c>
       <c r="AI1" s="4">
         <f t="shared" si="1"/>
-        <v>0.645</v>
+        <v>0.73</v>
       </c>
       <c r="AJ1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0.9333333333</v>
       </c>
       <c r="AK1" s="4">
         <f t="shared" si="1"/>
-        <v>0.78</v>
+        <v>0.9033333333</v>
       </c>
       <c r="AL1" s="4">
         <f t="shared" si="1"/>
-        <v>0.76</v>
+        <v>0.8733333333</v>
       </c>
       <c r="AM1" s="4">
         <f t="shared" si="1"/>
-        <v>0.59</v>
+        <v>0.6433333333</v>
       </c>
       <c r="AN1" s="4">
         <f t="shared" si="1"/>
-        <v>0.57</v>
+        <v>0.6133333333</v>
       </c>
       <c r="AO1" s="4">
         <f t="shared" si="1"/>
-        <v>0.675</v>
+        <v>0.75</v>
       </c>
       <c r="AP1" s="4">
         <f t="shared" si="1"/>
-        <v>0.83</v>
+        <v>0.9533333333</v>
       </c>
       <c r="AQ1" s="4">
         <f t="shared" si="1"/>
-        <v>0.81</v>
+        <v>0.9233333333</v>
       </c>
       <c r="AR1" s="4">
         <f t="shared" si="1"/>
-        <v>0.79</v>
+        <v>0.8933333333</v>
       </c>
       <c r="AS1" s="4">
         <f t="shared" si="1"/>
-        <v>0.62</v>
+        <v>0.6633333333</v>
       </c>
       <c r="AT1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>0.6333333333</v>
       </c>
       <c r="AU1" s="4">
         <f t="shared" si="1"/>
-        <v>0.705</v>
+        <v>0.77</v>
       </c>
       <c r="AV1" s="4">
         <f t="shared" si="1"/>
-        <v>0.86</v>
+        <v>0.9733333333</v>
       </c>
       <c r="AW1" s="4">
         <f t="shared" si="1"/>
-        <v>0.84</v>
+        <v>0.9433333333</v>
       </c>
       <c r="AX1" s="4">
         <f t="shared" si="1"/>
-        <v>0.82</v>
+        <v>0.9133333333</v>
       </c>
       <c r="AY1" s="4">
         <f t="shared" si="1"/>
-        <v>0.65</v>
+        <v>0.6833333333</v>
       </c>
       <c r="AZ1" s="4">
         <f t="shared" si="1"/>
-        <v>0.63</v>
+        <v>0.6533333333</v>
       </c>
       <c r="BA1" s="4">
         <f t="shared" si="1"/>
-        <v>0.735</v>
+        <v>0.79</v>
       </c>
       <c r="BB1" s="4">
         <f t="shared" si="1"/>
-        <v>0.89</v>
+        <v>0.9933333333</v>
       </c>
       <c r="BC1" s="4">
         <f t="shared" si="1"/>
-        <v>0.87</v>
+        <v>0.9633333333</v>
       </c>
       <c r="BD1" s="4">
         <f t="shared" si="1"/>
-        <v>0.85</v>
+        <v>0.9333333333</v>
       </c>
       <c r="BE1" s="4">
         <f t="shared" si="1"/>
-        <v>0.68</v>
+        <v>0.7033333333</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="5"/>
       <c r="E2" s="3"/>
       <c r="F2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(F9:F987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(F9:F984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="G2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(G9:G987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(G9:G984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="H2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(H9:H987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(H9:H984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="I2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(I9:I987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(I9:I984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="J2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(J9:J987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(J9:J984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="K2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(K9:K987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(K9:K984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="L2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(L9:L987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(L9:L984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="M2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(M9:M987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(M9:M984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="N2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(N9:N987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(N9:N984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="O2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(O9:O987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(O9:O984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="P2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(P9:P987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(P9:P984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="Q2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(Q9:Q987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(Q9:Q984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="R2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(R9:R987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(R9:R984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="S2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(S9:S987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(S9:S984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="T2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(T9:T987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(T9:T984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="U2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(U9:U987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(U9:U984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="V2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(V9:V987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(V9:V984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="W2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(W9:W987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(W9:W984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="X2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(X9:X987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(X9:X984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="Y2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(Y9:Y987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(Y9:Y984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="Z2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(Z9:Z987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(Z9:Z984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AA2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AA9:AA987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AA9:AA984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AB2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AB9:AB987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AB9:AB984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AC2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AC9:AC987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AC9:AC984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AD2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AD9:AD987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AD9:AD984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AE2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AE9:AE987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AE9:AE984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AF2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AF9:AF987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AF9:AF984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AG2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AG9:AG987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AG9:AG984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AH2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AH9:AH987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AH9:AH984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AI2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AI9:AI987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AI9:AI984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AJ2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AJ9:AJ987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AJ9:AJ984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AK2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AK9:AK987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AK9:AK984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AL2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AL9:AL987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AL9:AL984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AM2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AM9:AM987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AM9:AM984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AN2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AN9:AN987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AN9:AN984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AO2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AO9:AO987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AO9:AO984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AP2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AP9:AP987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AP9:AP984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AQ2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AQ9:AQ987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AQ9:AQ984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AR2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AR9:AR987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AR9:AR984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AS2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AS9:AS987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AS9:AS984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AT2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AT9:AT987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AT9:AT984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AU2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AU9:AU987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AU9:AU984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AV2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AV9:AV987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AV9:AV984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AW2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AW9:AW987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AW9:AW984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AX2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AX9:AX987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AX9:AX984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AY2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AY9:AY987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AY9:AY984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="AZ2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AZ9:AZ987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(AZ9:AZ984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="BA2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(BA9:BA987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(BA9:BA984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="BB2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(BB9:BB987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(BB9:BB984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="BC2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(BC9:BC987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(BC9:BC984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="BD2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(BD9:BD987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(BD9:BD984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
       <c r="BE2" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(BE9:BE987,$E9:$E987,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(AVERAGEIFS(BE9:BE984,$E9:$E984,""% Target""), {""charttype"",""column"";""ymin"",0%;""ymax"",100%;""color"",""green""})"),"")</f>
         <v/>
       </c>
     </row>
@@ -11996,7 +11982,7 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="20">
-        <f>SUMIFS(C10:C987,A10:A987,A10)</f>
+        <f>SUMIFS(C10:C984,A10:A984,A10)</f>
         <v>0.9112692308</v>
       </c>
       <c r="D9" s="21"/>
@@ -12059,7 +12045,7 @@
         <v>36</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C10" s="25">
         <f t="array" ref="C10">IF( B11="Short-Term", AVERAGE(F12:BE12)*B12, INDEX(F12:BE12, 1, COUNTA(F12:BE12))*B12 )</f>
@@ -12617,7 +12603,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C13" s="25">
         <f t="array" ref="C13">IF( B14="Short-Term", AVERAGE(F15:BE15)*B15, INDEX(F15:BE15, 1, COUNTA(F15:BE15))*B15 )</f>
@@ -13178,27 +13164,626 @@
       <c r="E16" s="8"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="31"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20">
+        <f>SUMIFS(C18:C984,A18:A984,A18)</f>
+        <v>0.4865384615</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+      <c r="V17" s="21"/>
+      <c r="W17" s="21"/>
+      <c r="X17" s="21"/>
+      <c r="Y17" s="21"/>
+      <c r="Z17" s="21"/>
+      <c r="AA17" s="21"/>
+      <c r="AB17" s="21"/>
+      <c r="AC17" s="21"/>
+      <c r="AD17" s="21"/>
+      <c r="AE17" s="21"/>
+      <c r="AF17" s="21"/>
+      <c r="AG17" s="21"/>
+      <c r="AH17" s="21"/>
+      <c r="AI17" s="21"/>
+      <c r="AJ17" s="21"/>
+      <c r="AK17" s="21"/>
+      <c r="AL17" s="21"/>
+      <c r="AM17" s="21"/>
+      <c r="AN17" s="21"/>
+      <c r="AO17" s="21"/>
+      <c r="AP17" s="21"/>
+      <c r="AQ17" s="21"/>
+      <c r="AR17" s="21"/>
+      <c r="AS17" s="21"/>
+      <c r="AT17" s="21"/>
+      <c r="AU17" s="21"/>
+      <c r="AV17" s="21"/>
+      <c r="AW17" s="21"/>
+      <c r="AX17" s="21"/>
+      <c r="AY17" s="21"/>
+      <c r="AZ17" s="21"/>
+      <c r="BA17" s="21"/>
+      <c r="BB17" s="21"/>
+      <c r="BC17" s="21"/>
+      <c r="BD17" s="21"/>
+      <c r="BE17" s="21"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="32"/>
+      <c r="A18" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="25">
+        <f t="array" ref="C18">IF( B19="Short-Term", AVERAGE(F20:BE20)*B20, INDEX(F20:BE20, 1, COUNTA(F20:BE20))*B20 )</f>
+        <v>0.4865384615</v>
+      </c>
+      <c r="D18" s="6" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B19=""Short-Term"", SPARKLINE(F20:BE20,IF(B18=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F20:BE20, 1, COUNTA(F20:BE20)) ,IF(B18=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
+        <v/>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="G18" s="33">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="H18" s="33">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="I18" s="33">
+        <v>0.625</v>
+      </c>
+      <c r="J18" s="33">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="K18" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="L18" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="M18" s="33">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="N18" s="33">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="O18" s="33">
+        <v>0.625</v>
+      </c>
+      <c r="P18" s="33">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="Q18" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="R18" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="S18" s="33">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="T18" s="33">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="U18" s="33">
+        <v>0.625</v>
+      </c>
+      <c r="V18" s="33">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="W18" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="X18" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="Y18" s="33">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="Z18" s="33">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="AA18" s="33">
+        <v>0.625</v>
+      </c>
+      <c r="AB18" s="33">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="AC18" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="AD18" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="AE18" s="33">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="AF18" s="33">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="AG18" s="33">
+        <v>0.625</v>
+      </c>
+      <c r="AH18" s="33">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="AI18" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="AJ18" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="AK18" s="33">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="AL18" s="33">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="AM18" s="33">
+        <v>0.625</v>
+      </c>
+      <c r="AN18" s="33">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="AO18" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="AP18" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="AQ18" s="33">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="AR18" s="33">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="AS18" s="33">
+        <v>0.625</v>
+      </c>
+      <c r="AT18" s="33">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="AU18" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="AV18" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="AW18" s="33">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="AX18" s="33">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="AY18" s="33">
+        <v>0.625</v>
+      </c>
+      <c r="AZ18" s="33">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="BA18" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="BB18" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="BC18" s="33">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="BD18" s="33">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="BE18" s="33">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="G19" s="35"/>
+      <c r="A19" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="G19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="H19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="I19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="J19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="K19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="L19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="M19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="N19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="O19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="P19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="Q19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="R19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="S19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="T19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="U19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="V19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="W19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="X19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="Y19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="Z19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AA19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AB19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AC19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AD19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AE19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AF19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AG19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AH19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AI19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AJ19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AK19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AL19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AM19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AN19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AO19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AP19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AQ19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AR19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AS19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AT19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AU19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AV19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AW19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AX19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AY19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="AZ19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="BA19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="BB19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="BC19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="BD19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="BE19" s="34">
+        <v>0.8333333333333334</v>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="B20" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="29">
+        <f t="shared" ref="F20:BE20" si="4">IF( $B18="Maximum", F18/F19 , IF( 100%-(F18-F19)/F19 &gt; 0, 100%-(F18-F19)/F19, 0) )</f>
+        <v>1.2</v>
+      </c>
+      <c r="G20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.15</v>
+      </c>
+      <c r="H20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.1</v>
+      </c>
+      <c r="I20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="J20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.7</v>
+      </c>
+      <c r="K20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.9</v>
+      </c>
+      <c r="L20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="M20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.15</v>
+      </c>
+      <c r="N20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.1</v>
+      </c>
+      <c r="O20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="P20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.7</v>
+      </c>
+      <c r="Q20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.9</v>
+      </c>
+      <c r="R20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="S20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.15</v>
+      </c>
+      <c r="T20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.1</v>
+      </c>
+      <c r="U20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="V20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.7</v>
+      </c>
+      <c r="W20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.9</v>
+      </c>
+      <c r="X20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="Y20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.15</v>
+      </c>
+      <c r="Z20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.1</v>
+      </c>
+      <c r="AA20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="AB20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.7</v>
+      </c>
+      <c r="AC20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.9</v>
+      </c>
+      <c r="AD20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="AE20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.15</v>
+      </c>
+      <c r="AF20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.1</v>
+      </c>
+      <c r="AG20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="AH20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.7</v>
+      </c>
+      <c r="AI20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.9</v>
+      </c>
+      <c r="AJ20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="AK20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.15</v>
+      </c>
+      <c r="AL20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.1</v>
+      </c>
+      <c r="AM20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="AN20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.7</v>
+      </c>
+      <c r="AO20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.9</v>
+      </c>
+      <c r="AP20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="AQ20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.15</v>
+      </c>
+      <c r="AR20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.1</v>
+      </c>
+      <c r="AS20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="AT20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.7</v>
+      </c>
+      <c r="AU20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.9</v>
+      </c>
+      <c r="AV20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="AW20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.15</v>
+      </c>
+      <c r="AX20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.1</v>
+      </c>
+      <c r="AY20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="AZ20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.7</v>
+      </c>
+      <c r="BA20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.9</v>
+      </c>
+      <c r="BB20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="BC20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.15</v>
+      </c>
+      <c r="BD20" s="29">
+        <f t="shared" si="4"/>
+        <v>1.1</v>
+      </c>
+      <c r="BE20" s="29">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="7"/>
@@ -18020,38 +18605,31 @@
       <c r="B984" s="8"/>
       <c r="E984" s="8"/>
     </row>
-    <row r="985" ht="15.75" customHeight="1">
-      <c r="A985" s="7"/>
-      <c r="B985" s="8"/>
-      <c r="E985" s="8"/>
-    </row>
-    <row r="986" ht="15.75" customHeight="1">
-      <c r="A986" s="7"/>
-      <c r="B986" s="8"/>
-      <c r="E986" s="8"/>
-    </row>
-    <row r="987" ht="15.75" customHeight="1">
-      <c r="A987" s="7"/>
-      <c r="B987" s="8"/>
-      <c r="E987" s="8"/>
-    </row>
   </sheetData>
-  <mergeCells count="71">
-    <mergeCell ref="AM2:AM4"/>
-    <mergeCell ref="AN2:AN4"/>
-    <mergeCell ref="AO2:AO4"/>
-    <mergeCell ref="AP2:AP4"/>
-    <mergeCell ref="AQ2:AQ4"/>
-    <mergeCell ref="AR2:AR4"/>
-    <mergeCell ref="AS2:AS4"/>
-    <mergeCell ref="AF2:AF4"/>
-    <mergeCell ref="AG2:AG4"/>
-    <mergeCell ref="AH2:AH4"/>
-    <mergeCell ref="AI2:AI4"/>
-    <mergeCell ref="AJ2:AJ4"/>
-    <mergeCell ref="AK2:AK4"/>
-    <mergeCell ref="AL2:AL4"/>
+  <mergeCells count="74">
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="Q2:Q4"/>
     <mergeCell ref="R2:R4"/>
+    <mergeCell ref="B1:D4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
     <mergeCell ref="S2:S4"/>
     <mergeCell ref="T2:T4"/>
     <mergeCell ref="U2:U4"/>
@@ -18065,10 +18643,20 @@
     <mergeCell ref="AC2:AC4"/>
     <mergeCell ref="AD2:AD4"/>
     <mergeCell ref="AE2:AE4"/>
-    <mergeCell ref="AW2:AW4"/>
-    <mergeCell ref="AX2:AX4"/>
-    <mergeCell ref="AY2:AY4"/>
-    <mergeCell ref="AZ2:AZ4"/>
+    <mergeCell ref="AF2:AF4"/>
+    <mergeCell ref="AG2:AG4"/>
+    <mergeCell ref="AH2:AH4"/>
+    <mergeCell ref="AI2:AI4"/>
+    <mergeCell ref="AJ2:AJ4"/>
+    <mergeCell ref="AK2:AK4"/>
+    <mergeCell ref="AL2:AL4"/>
+    <mergeCell ref="AM2:AM4"/>
+    <mergeCell ref="AN2:AN4"/>
+    <mergeCell ref="AO2:AO4"/>
+    <mergeCell ref="AP2:AP4"/>
+    <mergeCell ref="AQ2:AQ4"/>
+    <mergeCell ref="AR2:AR4"/>
+    <mergeCell ref="AS2:AS4"/>
     <mergeCell ref="AT2:AT4"/>
     <mergeCell ref="BB2:BB4"/>
     <mergeCell ref="BC2:BC4"/>
@@ -18076,59 +18664,44 @@
     <mergeCell ref="BE2:BE4"/>
     <mergeCell ref="AU2:AU4"/>
     <mergeCell ref="AV2:AV4"/>
+    <mergeCell ref="AW2:AW4"/>
+    <mergeCell ref="AX2:AX4"/>
+    <mergeCell ref="AY2:AY4"/>
+    <mergeCell ref="AZ2:AZ4"/>
     <mergeCell ref="BA2:BA4"/>
+    <mergeCell ref="AJ6:AN6"/>
     <mergeCell ref="AO6:AR6"/>
     <mergeCell ref="AS6:AW6"/>
     <mergeCell ref="AX6:BA6"/>
     <mergeCell ref="BB6:BE6"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="K6:N6"/>
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="W6:AA6"/>
     <mergeCell ref="AB6:AE6"/>
-    <mergeCell ref="AJ6:AN6"/>
     <mergeCell ref="AF6:AI6"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="P2:P4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B1:D4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="F6:J6"/>
   </mergeCells>
-  <conditionalFormatting sqref="F10:BE10 F13:BE13">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="F10:BE10 F13:BE13 F18:BE18">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND($B10="Maximum",F10&gt;=F11)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:BE10 F13:BE13">
-    <cfRule type="expression" dxfId="0" priority="2">
+  <conditionalFormatting sqref="F10:BE10 F13:BE13 F18:BE18">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND($B10="Minimum",50%&gt;F12)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:BE10 F13:BE13">
+  <conditionalFormatting sqref="F10:BE10 F13:BE13 F18:BE18">
     <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(F10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B10 B13">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B10 B13 B18">
       <formula1>"Maximum,Minimum"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B11 B14">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B11 B14 B19">
       <formula1>"Long-Term,Short-Term"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fix: BSC template drop down color not working
</commit_message>
<xml_diff>
--- a/templates/management/Balance Scorecard (BSC).xlsx
+++ b/templates/management/Balance Scorecard (BSC).xlsx
@@ -427,7 +427,7 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
     <dxf>
       <font/>
       <fill>
@@ -454,6 +454,36 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFF00"/>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAD1DC"/>
+          <bgColor rgb="FFEAD1DC"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
         </patternFill>
       </fill>
       <border/>
@@ -751,211 +781,211 @@
       <c r="E1" s="3"/>
       <c r="F1" s="4">
         <f t="shared" ref="F1:BE1" si="1">AVERAGEIFS(F9:F1013,$E9:$E1013,"% Target")</f>
-        <v>0.5476855879</v>
+        <v>0.5123800165</v>
       </c>
       <c r="G1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4958593407</v>
+        <v>0.5176367692</v>
       </c>
       <c r="H1" s="4">
         <f t="shared" si="1"/>
-        <v>0.3818893571</v>
+        <v>0.4607013571</v>
       </c>
       <c r="I1" s="4">
         <f t="shared" si="1"/>
-        <v>0.575169989</v>
+        <v>0.5576107033</v>
       </c>
       <c r="J1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5814697418</v>
+        <v>0.6340390275</v>
       </c>
       <c r="K1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4971453516</v>
+        <v>0.5459087802</v>
       </c>
       <c r="L1" s="4">
         <f t="shared" si="1"/>
-        <v>0.572833533</v>
+        <v>0.4412653901</v>
       </c>
       <c r="M1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5798191429</v>
+        <v>0.5587292857</v>
       </c>
       <c r="N1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5578983242</v>
+        <v>0.5151501813</v>
       </c>
       <c r="O1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5489223626</v>
+        <v>0.5058896484</v>
       </c>
       <c r="P1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6871329725</v>
+        <v>0.5449571154</v>
       </c>
       <c r="Q1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6182335824</v>
+        <v>0.508231011</v>
       </c>
       <c r="R1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4932197637</v>
+        <v>0.5315597637</v>
       </c>
       <c r="S1" s="4">
         <f t="shared" si="1"/>
-        <v>0.4935375165</v>
+        <v>0.6444495165</v>
       </c>
       <c r="T1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6285525549</v>
+        <v>0.5985019835</v>
       </c>
       <c r="U1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6043277363</v>
+        <v>0.6556178791</v>
       </c>
       <c r="V1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5898452033</v>
+        <v>0.625416489</v>
       </c>
       <c r="W1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7299640989</v>
+        <v>0.5915535275</v>
       </c>
       <c r="X1" s="4">
         <f t="shared" si="1"/>
-        <v>0.5666115659</v>
+        <v>0.6402661374</v>
       </c>
       <c r="Y1" s="4">
         <f t="shared" si="1"/>
-        <v>0.606244033</v>
+        <v>0.6167071758</v>
       </c>
       <c r="Z1" s="4">
         <f t="shared" si="1"/>
-        <v>0.6258436429</v>
+        <v>0.5973662143</v>
       </c>
       <c r="AA1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7588926813</v>
+        <v>0.7528155385</v>
       </c>
       <c r="AB1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7149505769</v>
+        <v>0.7932020055</v>
       </c>
       <c r="AC1" s="4">
         <f t="shared" si="1"/>
-        <v>0.809738044</v>
+        <v>0.6804049011</v>
       </c>
       <c r="AD1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7316729396</v>
+        <v>0.7140917967</v>
       </c>
       <c r="AE1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7580118352</v>
+        <v>0.7005654066</v>
       </c>
       <c r="AF1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7018445879</v>
+        <v>0.6387427308</v>
       </c>
       <c r="AG1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7790114835</v>
+        <v>0.7078747692</v>
       </c>
       <c r="AH1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7715890934</v>
+        <v>0.7918943791</v>
       </c>
       <c r="AI1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7752677033</v>
+        <v>0.7775055604</v>
       </c>
       <c r="AJ1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7765193132</v>
+        <v>0.7727668846</v>
       </c>
       <c r="AK1" s="4">
         <f t="shared" si="1"/>
-        <v>0.7806887802</v>
+        <v>0.7668852088</v>
       </c>
       <c r="AL1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8285609615</v>
+        <v>0.8124896758</v>
       </c>
       <c r="AM1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8736687143</v>
+        <v>0.8761102857</v>
       </c>
       <c r="AN1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8941190385</v>
+        <v>0.7823236099</v>
       </c>
       <c r="AO1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8578730769</v>
+        <v>0.8267819341</v>
       </c>
       <c r="AP1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9002958297</v>
+        <v>0.868796544</v>
       </c>
       <c r="AQ1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8326777253</v>
+        <v>0.8915434396</v>
       </c>
       <c r="AR1" s="4">
         <f t="shared" si="1"/>
-        <v>0.8648131923</v>
+        <v>0.826209478</v>
       </c>
       <c r="AS1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9090312308</v>
+        <v>0.9499948022</v>
       </c>
       <c r="AT1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9869829835</v>
+        <v>0.9284955549</v>
       </c>
       <c r="AU1" s="4">
         <f t="shared" si="1"/>
-        <v>0.926104022</v>
+        <v>0.9715573077</v>
       </c>
       <c r="AV1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9530286319</v>
+        <v>0.9195082033</v>
       </c>
       <c r="AW1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9556492418</v>
+        <v>0.9499325275</v>
       </c>
       <c r="AX1" s="4">
         <f t="shared" si="1"/>
-        <v>0.9719321374</v>
+        <v>0.9156012802</v>
       </c>
       <c r="AY1" s="4">
         <f t="shared" si="1"/>
-        <v>1.07047889</v>
+        <v>1.125087604</v>
       </c>
       <c r="AZ1" s="4">
         <f t="shared" si="1"/>
-        <v>1.112661643</v>
+        <v>1.030659357</v>
       </c>
       <c r="BA1" s="4">
         <f t="shared" si="1"/>
-        <v>1.071864396</v>
+        <v>1.071155253</v>
       </c>
       <c r="BB1" s="4">
         <f t="shared" si="1"/>
-        <v>1.027063577</v>
+        <v>1.089324863</v>
       </c>
       <c r="BC1" s="4">
         <f t="shared" si="1"/>
-        <v>1.062574187</v>
+        <v>0.963132044</v>
       </c>
       <c r="BD1" s="4">
         <f t="shared" si="1"/>
-        <v>1.063307797</v>
+        <v>0.9902587967</v>
       </c>
       <c r="BE1" s="4">
         <f t="shared" si="1"/>
-        <v>1.102497264</v>
+        <v>1.172712549</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -1411,7 +1441,7 @@
       <c r="B9" s="19"/>
       <c r="C9" s="20">
         <f>SUMIFS(C10:C1013,A10:A1013,A10)</f>
-        <v>0.9026899011</v>
+        <v>0.902465156</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="22"/>
@@ -1477,7 +1507,7 @@
       </c>
       <c r="C10" s="25">
         <f t="array" ref="C10">IF( B11="Short-Term", AVERAGE(F12:BE12)*B12, INDEX(F12:BE12, 1, COUNTA(F12:BE12))*B12 )</f>
-        <v>0.3030948462</v>
+        <v>0.3081404308</v>
       </c>
       <c r="D10" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B11=""Short-Term"", SPARKLINE(F12:BE12,IF(B10=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F12:BE12, 1, COUNTA(F12:BE12)) ,IF(B10=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -1488,211 +1518,211 @@
       </c>
       <c r="F10" s="26">
         <f t="shared" ref="F10:BE10" si="2">RANDBETWEEN(100000,150000)</f>
-        <v>131164</v>
+        <v>135416</v>
       </c>
       <c r="G10" s="26">
         <f t="shared" si="2"/>
-        <v>131550</v>
+        <v>116094</v>
       </c>
       <c r="H10" s="26">
         <f t="shared" si="2"/>
-        <v>145441</v>
+        <v>112629</v>
       </c>
       <c r="I10" s="26">
         <f t="shared" si="2"/>
-        <v>122341</v>
+        <v>119311</v>
       </c>
       <c r="J10" s="26">
         <f t="shared" si="2"/>
-        <v>147101</v>
+        <v>104996</v>
       </c>
       <c r="K10" s="26">
         <f t="shared" si="2"/>
-        <v>130253</v>
+        <v>111186</v>
       </c>
       <c r="L10" s="26">
         <f t="shared" si="2"/>
-        <v>106321</v>
+        <v>133532</v>
       </c>
       <c r="M10" s="26">
         <f t="shared" si="2"/>
-        <v>103413</v>
+        <v>100985</v>
       </c>
       <c r="N10" s="26">
         <f t="shared" si="2"/>
-        <v>112715</v>
+        <v>140481</v>
       </c>
       <c r="O10" s="26">
         <f t="shared" si="2"/>
-        <v>105340</v>
+        <v>116587</v>
       </c>
       <c r="P10" s="26">
         <f t="shared" si="2"/>
-        <v>107207</v>
+        <v>118240</v>
       </c>
       <c r="Q10" s="26">
         <f t="shared" si="2"/>
-        <v>110184</v>
+        <v>120633</v>
       </c>
       <c r="R10" s="26">
         <f t="shared" si="2"/>
-        <v>128704</v>
+        <v>117739</v>
       </c>
       <c r="S10" s="26">
         <f t="shared" si="2"/>
-        <v>116321</v>
+        <v>102284</v>
       </c>
       <c r="T10" s="26">
         <f t="shared" si="2"/>
-        <v>141955</v>
+        <v>130827</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="2"/>
-        <v>119061</v>
+        <v>118003</v>
       </c>
       <c r="V10" s="26">
         <f t="shared" si="2"/>
-        <v>140264</v>
+        <v>119907</v>
       </c>
       <c r="W10" s="26">
         <f t="shared" si="2"/>
-        <v>116562</v>
+        <v>148419</v>
       </c>
       <c r="X10" s="26">
         <f t="shared" si="2"/>
-        <v>123635</v>
+        <v>120784</v>
       </c>
       <c r="Y10" s="26">
         <f t="shared" si="2"/>
-        <v>121473</v>
+        <v>117367</v>
       </c>
       <c r="Z10" s="26">
         <f t="shared" si="2"/>
-        <v>112076</v>
+        <v>147482</v>
       </c>
       <c r="AA10" s="26">
         <f t="shared" si="2"/>
-        <v>123301</v>
+        <v>111771</v>
       </c>
       <c r="AB10" s="26">
         <f t="shared" si="2"/>
-        <v>138785</v>
+        <v>114105</v>
       </c>
       <c r="AC10" s="26">
         <f t="shared" si="2"/>
-        <v>134218</v>
+        <v>113694</v>
       </c>
       <c r="AD10" s="26">
         <f t="shared" si="2"/>
-        <v>115450</v>
+        <v>111299</v>
       </c>
       <c r="AE10" s="26">
         <f t="shared" si="2"/>
-        <v>139403</v>
+        <v>125778</v>
       </c>
       <c r="AF10" s="26">
         <f t="shared" si="2"/>
-        <v>134505</v>
+        <v>118339</v>
       </c>
       <c r="AG10" s="26">
         <f t="shared" si="2"/>
-        <v>104880</v>
+        <v>118981</v>
       </c>
       <c r="AH10" s="26">
         <f t="shared" si="2"/>
-        <v>121755</v>
+        <v>125789</v>
       </c>
       <c r="AI10" s="26">
         <f t="shared" si="2"/>
-        <v>133154</v>
+        <v>113309</v>
       </c>
       <c r="AJ10" s="26">
         <f t="shared" si="2"/>
-        <v>128855</v>
+        <v>124286</v>
       </c>
       <c r="AK10" s="26">
         <f t="shared" si="2"/>
-        <v>144031</v>
+        <v>112656</v>
       </c>
       <c r="AL10" s="26">
         <f t="shared" si="2"/>
-        <v>123665</v>
+        <v>138272</v>
       </c>
       <c r="AM10" s="26">
         <f t="shared" si="2"/>
-        <v>133617</v>
+        <v>149354</v>
       </c>
       <c r="AN10" s="26">
         <f t="shared" si="2"/>
-        <v>138155</v>
+        <v>137379</v>
       </c>
       <c r="AO10" s="26">
         <f t="shared" si="2"/>
-        <v>124175</v>
+        <v>111159</v>
       </c>
       <c r="AP10" s="26">
         <f t="shared" si="2"/>
-        <v>147187</v>
+        <v>125097</v>
       </c>
       <c r="AQ10" s="26">
         <f t="shared" si="2"/>
-        <v>126847</v>
+        <v>107642</v>
       </c>
       <c r="AR10" s="26">
         <f t="shared" si="2"/>
-        <v>107057</v>
+        <v>123875</v>
       </c>
       <c r="AS10" s="26">
         <f t="shared" si="2"/>
-        <v>145238</v>
+        <v>106953</v>
       </c>
       <c r="AT10" s="26">
         <f t="shared" si="2"/>
-        <v>122971</v>
+        <v>106887</v>
       </c>
       <c r="AU10" s="26">
         <f t="shared" si="2"/>
-        <v>142624</v>
+        <v>111260</v>
       </c>
       <c r="AV10" s="26">
         <f t="shared" si="2"/>
-        <v>108527</v>
+        <v>110476</v>
       </c>
       <c r="AW10" s="26">
         <f t="shared" si="2"/>
-        <v>127734</v>
+        <v>126540</v>
       </c>
       <c r="AX10" s="26">
         <f t="shared" si="2"/>
-        <v>104993</v>
+        <v>133306</v>
       </c>
       <c r="AY10" s="26">
         <f t="shared" si="2"/>
-        <v>102256</v>
+        <v>132308</v>
       </c>
       <c r="AZ10" s="26">
         <f t="shared" si="2"/>
-        <v>101258</v>
+        <v>131171</v>
       </c>
       <c r="BA10" s="26">
         <f t="shared" si="2"/>
-        <v>107740</v>
+        <v>120342</v>
       </c>
       <c r="BB10" s="26">
         <f t="shared" si="2"/>
-        <v>108297</v>
+        <v>112375</v>
       </c>
       <c r="BC10" s="26">
         <f t="shared" si="2"/>
-        <v>105489</v>
+        <v>149824</v>
       </c>
       <c r="BD10" s="26">
         <f t="shared" si="2"/>
-        <v>141458</v>
+        <v>121757</v>
       </c>
       <c r="BE10" s="26">
         <f t="shared" si="2"/>
-        <v>122239</v>
+        <v>124738</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -1871,211 +1901,211 @@
       </c>
       <c r="F12" s="29">
         <f t="shared" ref="F12:BE12" si="3">IF( $B10="Maximum", F10/F11 , IF( 100%-(F10-F11)/F11 &gt; 0, 100%-(F10-F11)/F11, 0) )</f>
-        <v>0.950688</v>
+        <v>0.916672</v>
       </c>
       <c r="G12" s="29">
         <f t="shared" si="3"/>
-        <v>0.9476</v>
+        <v>1.071248</v>
       </c>
       <c r="H12" s="29">
         <f t="shared" si="3"/>
-        <v>0.836472</v>
+        <v>1.098968</v>
       </c>
       <c r="I12" s="29">
         <f t="shared" si="3"/>
-        <v>1.021272</v>
+        <v>1.045512</v>
       </c>
       <c r="J12" s="29">
         <f t="shared" si="3"/>
-        <v>0.823192</v>
+        <v>1.160032</v>
       </c>
       <c r="K12" s="29">
         <f t="shared" si="3"/>
-        <v>0.957976</v>
+        <v>1.110512</v>
       </c>
       <c r="L12" s="29">
         <f t="shared" si="3"/>
-        <v>1.149432</v>
+        <v>0.931744</v>
       </c>
       <c r="M12" s="29">
         <f t="shared" si="3"/>
-        <v>1.172696</v>
+        <v>1.19212</v>
       </c>
       <c r="N12" s="29">
         <f t="shared" si="3"/>
-        <v>1.09828</v>
+        <v>0.876152</v>
       </c>
       <c r="O12" s="29">
         <f t="shared" si="3"/>
-        <v>1.15728</v>
+        <v>1.067304</v>
       </c>
       <c r="P12" s="29">
         <f t="shared" si="3"/>
-        <v>1.142344</v>
+        <v>1.05408</v>
       </c>
       <c r="Q12" s="29">
         <f t="shared" si="3"/>
-        <v>1.118528</v>
+        <v>1.034936</v>
       </c>
       <c r="R12" s="29">
         <f t="shared" si="3"/>
-        <v>0.970368</v>
+        <v>1.058088</v>
       </c>
       <c r="S12" s="29">
         <f t="shared" si="3"/>
-        <v>1.069432</v>
+        <v>1.181728</v>
       </c>
       <c r="T12" s="29">
         <f t="shared" si="3"/>
-        <v>0.86436</v>
+        <v>0.953384</v>
       </c>
       <c r="U12" s="29">
         <f t="shared" si="3"/>
-        <v>1.047512</v>
+        <v>1.055976</v>
       </c>
       <c r="V12" s="29">
         <f t="shared" si="3"/>
-        <v>0.877888</v>
+        <v>1.040744</v>
       </c>
       <c r="W12" s="29">
         <f t="shared" si="3"/>
-        <v>1.067504</v>
+        <v>0.812648</v>
       </c>
       <c r="X12" s="29">
         <f t="shared" si="3"/>
-        <v>1.01092</v>
+        <v>1.033728</v>
       </c>
       <c r="Y12" s="29">
         <f t="shared" si="3"/>
-        <v>1.028216</v>
+        <v>1.061064</v>
       </c>
       <c r="Z12" s="29">
         <f t="shared" si="3"/>
-        <v>1.103392</v>
+        <v>0.820144</v>
       </c>
       <c r="AA12" s="29">
         <f t="shared" si="3"/>
-        <v>1.013592</v>
+        <v>1.105832</v>
       </c>
       <c r="AB12" s="29">
         <f t="shared" si="3"/>
-        <v>0.88972</v>
+        <v>1.08716</v>
       </c>
       <c r="AC12" s="29">
         <f t="shared" si="3"/>
-        <v>0.926256</v>
+        <v>1.090448</v>
       </c>
       <c r="AD12" s="29">
         <f t="shared" si="3"/>
-        <v>1.0764</v>
+        <v>1.109608</v>
       </c>
       <c r="AE12" s="29">
         <f t="shared" si="3"/>
-        <v>0.884776</v>
+        <v>0.993776</v>
       </c>
       <c r="AF12" s="29">
         <f t="shared" si="3"/>
-        <v>0.92396</v>
+        <v>1.053288</v>
       </c>
       <c r="AG12" s="29">
         <f t="shared" si="3"/>
-        <v>1.16096</v>
+        <v>1.048152</v>
       </c>
       <c r="AH12" s="29">
         <f t="shared" si="3"/>
-        <v>1.02596</v>
+        <v>0.993688</v>
       </c>
       <c r="AI12" s="29">
         <f t="shared" si="3"/>
-        <v>0.934768</v>
+        <v>1.093528</v>
       </c>
       <c r="AJ12" s="29">
         <f t="shared" si="3"/>
-        <v>0.96916</v>
+        <v>1.005712</v>
       </c>
       <c r="AK12" s="29">
         <f t="shared" si="3"/>
-        <v>0.847752</v>
+        <v>1.098752</v>
       </c>
       <c r="AL12" s="29">
         <f t="shared" si="3"/>
-        <v>1.01068</v>
+        <v>0.893824</v>
       </c>
       <c r="AM12" s="29">
         <f t="shared" si="3"/>
-        <v>0.931064</v>
+        <v>0.805168</v>
       </c>
       <c r="AN12" s="29">
         <f t="shared" si="3"/>
-        <v>0.89476</v>
+        <v>0.900968</v>
       </c>
       <c r="AO12" s="29">
         <f t="shared" si="3"/>
-        <v>1.0066</v>
+        <v>1.110728</v>
       </c>
       <c r="AP12" s="29">
         <f t="shared" si="3"/>
-        <v>0.822504</v>
+        <v>0.999224</v>
       </c>
       <c r="AQ12" s="29">
         <f t="shared" si="3"/>
-        <v>0.985224</v>
+        <v>1.138864</v>
       </c>
       <c r="AR12" s="29">
         <f t="shared" si="3"/>
-        <v>1.143544</v>
+        <v>1.009</v>
       </c>
       <c r="AS12" s="29">
         <f t="shared" si="3"/>
-        <v>0.838096</v>
+        <v>1.144376</v>
       </c>
       <c r="AT12" s="29">
         <f t="shared" si="3"/>
-        <v>1.016232</v>
+        <v>1.144904</v>
       </c>
       <c r="AU12" s="29">
         <f t="shared" si="3"/>
-        <v>0.859008</v>
+        <v>1.10992</v>
       </c>
       <c r="AV12" s="29">
         <f t="shared" si="3"/>
-        <v>1.131784</v>
+        <v>1.116192</v>
       </c>
       <c r="AW12" s="29">
         <f t="shared" si="3"/>
-        <v>0.978128</v>
+        <v>0.98768</v>
       </c>
       <c r="AX12" s="29">
         <f t="shared" si="3"/>
-        <v>1.160056</v>
+        <v>0.933552</v>
       </c>
       <c r="AY12" s="29">
         <f t="shared" si="3"/>
-        <v>1.181952</v>
+        <v>0.941536</v>
       </c>
       <c r="AZ12" s="29">
         <f t="shared" si="3"/>
-        <v>1.189936</v>
+        <v>0.950632</v>
       </c>
       <c r="BA12" s="29">
         <f t="shared" si="3"/>
-        <v>1.13808</v>
+        <v>1.037264</v>
       </c>
       <c r="BB12" s="29">
         <f t="shared" si="3"/>
-        <v>1.133624</v>
+        <v>1.101</v>
       </c>
       <c r="BC12" s="29">
         <f t="shared" si="3"/>
-        <v>1.156088</v>
+        <v>0.801408</v>
       </c>
       <c r="BD12" s="29">
         <f t="shared" si="3"/>
-        <v>0.868336</v>
+        <v>1.025944</v>
       </c>
       <c r="BE12" s="29">
         <f t="shared" si="3"/>
-        <v>1.022088</v>
+        <v>1.002096</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -2087,7 +2117,7 @@
       </c>
       <c r="C13" s="25">
         <f t="array" ref="C13">IF( B14="Short-Term", AVERAGE(F15:BE15)*B15, INDEX(F15:BE15, 1, COUNTA(F15:BE15))*B15 )</f>
-        <v>0.1897489011</v>
+        <v>0.1844785714</v>
       </c>
       <c r="D13" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B14=""Short-Term"", SPARKLINE(F15:BE15,IF(B13=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F15:BE15, 1, COUNTA(F15:BE15)) ,IF(B13=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -2098,211 +2128,211 @@
       </c>
       <c r="F13" s="26">
         <f t="shared" ref="F13:BE13" si="4">RANDBETWEEN(5000,10000)</f>
-        <v>8525</v>
+        <v>6064</v>
       </c>
       <c r="G13" s="26">
         <f t="shared" si="4"/>
-        <v>6857</v>
+        <v>7833</v>
       </c>
       <c r="H13" s="26">
         <f t="shared" si="4"/>
-        <v>9442</v>
+        <v>7076</v>
       </c>
       <c r="I13" s="26">
         <f t="shared" si="4"/>
-        <v>8954</v>
+        <v>7797</v>
       </c>
       <c r="J13" s="26">
         <f t="shared" si="4"/>
-        <v>7146</v>
+        <v>7820</v>
       </c>
       <c r="K13" s="26">
         <f t="shared" si="4"/>
-        <v>8613</v>
+        <v>7160</v>
       </c>
       <c r="L13" s="26">
         <f t="shared" si="4"/>
-        <v>7886</v>
+        <v>9530</v>
       </c>
       <c r="M13" s="26">
         <f t="shared" si="4"/>
-        <v>5699</v>
+        <v>7716</v>
       </c>
       <c r="N13" s="26">
         <f t="shared" si="4"/>
-        <v>5847</v>
+        <v>5706</v>
       </c>
       <c r="O13" s="26">
         <f t="shared" si="4"/>
-        <v>7674</v>
+        <v>8754</v>
       </c>
       <c r="P13" s="26">
         <f t="shared" si="4"/>
-        <v>5361</v>
+        <v>7175</v>
       </c>
       <c r="Q13" s="26">
         <f t="shared" si="4"/>
-        <v>5764</v>
+        <v>8329</v>
       </c>
       <c r="R13" s="26">
         <f t="shared" si="4"/>
-        <v>8999</v>
+        <v>6206</v>
       </c>
       <c r="S13" s="26">
         <f t="shared" si="4"/>
-        <v>8556</v>
+        <v>7051</v>
       </c>
       <c r="T13" s="26">
         <f t="shared" si="4"/>
-        <v>7191</v>
+        <v>6417</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="4"/>
-        <v>8781</v>
+        <v>6458</v>
       </c>
       <c r="V13" s="26">
         <f t="shared" si="4"/>
-        <v>8266</v>
+        <v>8114</v>
       </c>
       <c r="W13" s="26">
         <f t="shared" si="4"/>
-        <v>5808</v>
+        <v>6665</v>
       </c>
       <c r="X13" s="26">
         <f t="shared" si="4"/>
-        <v>8331</v>
+        <v>5766</v>
       </c>
       <c r="Y13" s="26">
         <f t="shared" si="4"/>
-        <v>9034</v>
+        <v>6648</v>
       </c>
       <c r="Z13" s="26">
         <f t="shared" si="4"/>
-        <v>9024</v>
+        <v>7586</v>
       </c>
       <c r="AA13" s="26">
         <f t="shared" si="4"/>
-        <v>6546</v>
+        <v>8652</v>
       </c>
       <c r="AB13" s="26">
         <f t="shared" si="4"/>
-        <v>5691</v>
+        <v>7031</v>
       </c>
       <c r="AC13" s="26">
         <f t="shared" si="4"/>
-        <v>5190</v>
+        <v>5812</v>
       </c>
       <c r="AD13" s="26">
         <f t="shared" si="4"/>
-        <v>6204</v>
+        <v>7351</v>
       </c>
       <c r="AE13" s="26">
         <f t="shared" si="4"/>
-        <v>5559</v>
+        <v>6669</v>
       </c>
       <c r="AF13" s="26">
         <f t="shared" si="4"/>
-        <v>8280</v>
+        <v>8449</v>
       </c>
       <c r="AG13" s="26">
         <f t="shared" si="4"/>
-        <v>9819</v>
+        <v>8113</v>
       </c>
       <c r="AH13" s="26">
         <f t="shared" si="4"/>
-        <v>9291</v>
+        <v>7928</v>
       </c>
       <c r="AI13" s="26">
         <f t="shared" si="4"/>
-        <v>7398</v>
+        <v>5864</v>
       </c>
       <c r="AJ13" s="26">
         <f t="shared" si="4"/>
-        <v>7990</v>
+        <v>5796</v>
       </c>
       <c r="AK13" s="26">
         <f t="shared" si="4"/>
-        <v>9778</v>
+        <v>6638</v>
       </c>
       <c r="AL13" s="26">
         <f t="shared" si="4"/>
-        <v>7189</v>
+        <v>5101</v>
       </c>
       <c r="AM13" s="26">
         <f t="shared" si="4"/>
-        <v>9497</v>
+        <v>8899</v>
       </c>
       <c r="AN13" s="26">
         <f t="shared" si="4"/>
-        <v>5019</v>
+        <v>9573</v>
       </c>
       <c r="AO13" s="26">
         <f t="shared" si="4"/>
-        <v>6433</v>
+        <v>8833</v>
       </c>
       <c r="AP13" s="26">
         <f t="shared" si="4"/>
-        <v>6130</v>
+        <v>6891</v>
       </c>
       <c r="AQ13" s="26">
         <f t="shared" si="4"/>
-        <v>7697</v>
+        <v>8976</v>
       </c>
       <c r="AR13" s="26">
         <f t="shared" si="4"/>
-        <v>6867</v>
+        <v>8577</v>
       </c>
       <c r="AS13" s="26">
         <f t="shared" si="4"/>
-        <v>7644</v>
+        <v>9454</v>
       </c>
       <c r="AT13" s="26">
         <f t="shared" si="4"/>
-        <v>7607</v>
+        <v>9963</v>
       </c>
       <c r="AU13" s="26">
         <f t="shared" si="4"/>
-        <v>5507</v>
+        <v>9128</v>
       </c>
       <c r="AV13" s="26">
         <f t="shared" si="4"/>
-        <v>8780</v>
+        <v>7608</v>
       </c>
       <c r="AW13" s="26">
         <f t="shared" si="4"/>
-        <v>6649</v>
+        <v>8016</v>
       </c>
       <c r="AX13" s="26">
         <f t="shared" si="4"/>
-        <v>8552</v>
+        <v>9771</v>
       </c>
       <c r="AY13" s="26">
         <f t="shared" si="4"/>
-        <v>6058</v>
+        <v>5307</v>
       </c>
       <c r="AZ13" s="26">
         <f t="shared" si="4"/>
-        <v>6343</v>
+        <v>9540</v>
       </c>
       <c r="BA13" s="26">
         <f t="shared" si="4"/>
-        <v>6306</v>
+        <v>7320</v>
       </c>
       <c r="BB13" s="26">
         <f t="shared" si="4"/>
-        <v>7665</v>
+        <v>5700</v>
       </c>
       <c r="BC13" s="26">
         <f t="shared" si="4"/>
-        <v>5975</v>
+        <v>8011</v>
       </c>
       <c r="BD13" s="26">
         <f t="shared" si="4"/>
-        <v>7631</v>
+        <v>9745</v>
       </c>
       <c r="BE13" s="26">
         <f t="shared" si="4"/>
-        <v>5604</v>
+        <v>5662</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
@@ -2481,211 +2511,211 @@
       </c>
       <c r="F15" s="29">
         <f t="shared" ref="F15:BE15" si="5">IF( $B13="Maximum", F13/F14 , IF( 100%-(F13-F14)/F14 &gt; 0, 100%-(F13-F14)/F14, 0) )</f>
-        <v>0.7821428571</v>
+        <v>1.133714286</v>
       </c>
       <c r="G15" s="29">
         <f t="shared" si="5"/>
-        <v>1.020428571</v>
+        <v>0.881</v>
       </c>
       <c r="H15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6511428571</v>
+        <v>0.9891428571</v>
       </c>
       <c r="I15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7208571429</v>
+        <v>0.8861428571</v>
       </c>
       <c r="J15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9791428571</v>
+        <v>0.8828571429</v>
       </c>
       <c r="K15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7695714286</v>
+        <v>0.9771428571</v>
       </c>
       <c r="L15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8734285714</v>
+        <v>0.6385714286</v>
       </c>
       <c r="M15" s="29">
         <f t="shared" si="5"/>
-        <v>1.185857143</v>
+        <v>0.8977142857</v>
       </c>
       <c r="N15" s="29">
         <f t="shared" si="5"/>
-        <v>1.164714286</v>
+        <v>1.184857143</v>
       </c>
       <c r="O15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9037142857</v>
+        <v>0.7494285714</v>
       </c>
       <c r="P15" s="29">
         <f t="shared" si="5"/>
-        <v>1.234142857</v>
+        <v>0.975</v>
       </c>
       <c r="Q15" s="29">
         <f t="shared" si="5"/>
-        <v>1.176571429</v>
+        <v>0.8101428571</v>
       </c>
       <c r="R15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7144285714</v>
+        <v>1.113428571</v>
       </c>
       <c r="S15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7777142857</v>
+        <v>0.9927142857</v>
       </c>
       <c r="T15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9727142857</v>
+        <v>1.083285714</v>
       </c>
       <c r="U15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7455714286</v>
+        <v>1.077428571</v>
       </c>
       <c r="V15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8191428571</v>
+        <v>0.8408571429</v>
       </c>
       <c r="W15" s="29">
         <f t="shared" si="5"/>
-        <v>1.170285714</v>
+        <v>1.047857143</v>
       </c>
       <c r="X15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8098571429</v>
+        <v>1.176285714</v>
       </c>
       <c r="Y15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7094285714</v>
+        <v>1.050285714</v>
       </c>
       <c r="Z15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7108571429</v>
+        <v>0.9162857143</v>
       </c>
       <c r="AA15" s="29">
         <f t="shared" si="5"/>
-        <v>1.064857143</v>
+        <v>0.764</v>
       </c>
       <c r="AB15" s="29">
         <f t="shared" si="5"/>
-        <v>1.187</v>
+        <v>0.9955714286</v>
       </c>
       <c r="AC15" s="29">
         <f t="shared" si="5"/>
-        <v>1.258571429</v>
+        <v>1.169714286</v>
       </c>
       <c r="AD15" s="29">
         <f t="shared" si="5"/>
-        <v>1.113714286</v>
+        <v>0.9498571429</v>
       </c>
       <c r="AE15" s="29">
         <f t="shared" si="5"/>
-        <v>1.205857143</v>
+        <v>1.047285714</v>
       </c>
       <c r="AF15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8171428571</v>
+        <v>0.793</v>
       </c>
       <c r="AG15" s="29">
         <f t="shared" si="5"/>
-        <v>0.5972857143</v>
+        <v>0.841</v>
       </c>
       <c r="AH15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6727142857</v>
+        <v>0.8674285714</v>
       </c>
       <c r="AI15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9431428571</v>
+        <v>1.162285714</v>
       </c>
       <c r="AJ15" s="29">
         <f t="shared" si="5"/>
-        <v>0.8585714286</v>
+        <v>1.172</v>
       </c>
       <c r="AK15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6031428571</v>
+        <v>1.051714286</v>
       </c>
       <c r="AL15" s="29">
         <f t="shared" si="5"/>
-        <v>0.973</v>
+        <v>1.271285714</v>
       </c>
       <c r="AM15" s="29">
         <f t="shared" si="5"/>
-        <v>0.6432857143</v>
+        <v>0.7287142857</v>
       </c>
       <c r="AN15" s="29">
         <f t="shared" si="5"/>
-        <v>1.283</v>
+        <v>0.6324285714</v>
       </c>
       <c r="AO15" s="29">
         <f t="shared" si="5"/>
-        <v>1.081</v>
+        <v>0.7381428571</v>
       </c>
       <c r="AP15" s="29">
         <f t="shared" si="5"/>
-        <v>1.124285714</v>
+        <v>1.015571429</v>
       </c>
       <c r="AQ15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9004285714</v>
+        <v>0.7177142857</v>
       </c>
       <c r="AR15" s="29">
         <f t="shared" si="5"/>
-        <v>1.019</v>
+        <v>0.7747142857</v>
       </c>
       <c r="AS15" s="29">
         <f t="shared" si="5"/>
-        <v>0.908</v>
+        <v>0.6494285714</v>
       </c>
       <c r="AT15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9132857143</v>
+        <v>0.5767142857</v>
       </c>
       <c r="AU15" s="29">
         <f t="shared" si="5"/>
-        <v>1.213285714</v>
+        <v>0.696</v>
       </c>
       <c r="AV15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7457142857</v>
+        <v>0.9131428571</v>
       </c>
       <c r="AW15" s="29">
         <f t="shared" si="5"/>
-        <v>1.050142857</v>
+        <v>0.8548571429</v>
       </c>
       <c r="AX15" s="29">
         <f t="shared" si="5"/>
-        <v>0.7782857143</v>
+        <v>0.6041428571</v>
       </c>
       <c r="AY15" s="29">
         <f t="shared" si="5"/>
-        <v>1.134571429</v>
+        <v>1.241857143</v>
       </c>
       <c r="AZ15" s="29">
         <f t="shared" si="5"/>
-        <v>1.093857143</v>
+        <v>0.6371428571</v>
       </c>
       <c r="BA15" s="29">
         <f t="shared" si="5"/>
-        <v>1.099142857</v>
+        <v>0.9542857143</v>
       </c>
       <c r="BB15" s="29">
         <f t="shared" si="5"/>
-        <v>0.905</v>
+        <v>1.185714286</v>
       </c>
       <c r="BC15" s="29">
         <f t="shared" si="5"/>
-        <v>1.146428571</v>
+        <v>0.8555714286</v>
       </c>
       <c r="BD15" s="29">
         <f t="shared" si="5"/>
-        <v>0.9098571429</v>
+        <v>0.6078571429</v>
       </c>
       <c r="BE15" s="29">
         <f t="shared" si="5"/>
-        <v>1.199428571</v>
+        <v>1.191142857</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -4461,7 +4491,7 @@
       <c r="B30" s="19"/>
       <c r="C30" s="20">
         <f>SUMIFS(C31:C1013,A31:A1013,A31)</f>
-        <v>0.7341730769</v>
+        <v>0.6650769231</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
@@ -4527,7 +4557,7 @@
       </c>
       <c r="C31" s="25">
         <f t="array" ref="C31">IF( B32="Short-Term", AVERAGE(F33:BE33)*B33, INDEX(F33:BE33, 1, COUNTA(F33:BE33))*B33 )</f>
-        <v>0.3755769231</v>
+        <v>0.3071923077</v>
       </c>
       <c r="D31" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B32=""Short-Term"", SPARKLINE(F33:BE33,IF(B31=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F33:BE33, 1, COUNTA(F33:BE33)) ,IF(B31=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -4538,211 +4568,211 @@
       </c>
       <c r="F31" s="26">
         <f t="shared" ref="F31:BE31" si="9">RANDBETWEEN(1,50)</f>
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="G31" s="26">
         <f t="shared" si="9"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H31" s="26">
         <f t="shared" si="9"/>
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I31" s="26">
         <f t="shared" si="9"/>
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="J31" s="26">
         <f t="shared" si="9"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="K31" s="26">
         <f t="shared" si="9"/>
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="L31" s="26">
         <f t="shared" si="9"/>
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M31" s="26">
         <f t="shared" si="9"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N31" s="26">
         <f t="shared" si="9"/>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="O31" s="26">
         <f t="shared" si="9"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="P31" s="26">
         <f t="shared" si="9"/>
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="Q31" s="26">
         <f t="shared" si="9"/>
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="R31" s="26">
         <f t="shared" si="9"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="S31" s="26">
         <f t="shared" si="9"/>
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="T31" s="26">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="U31" s="26">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="V31" s="26">
         <f t="shared" si="9"/>
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="W31" s="26">
         <f t="shared" si="9"/>
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="X31" s="26">
         <f t="shared" si="9"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y31" s="26">
         <f t="shared" si="9"/>
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="Z31" s="26">
         <f t="shared" si="9"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AA31" s="26">
         <f t="shared" si="9"/>
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="AB31" s="26">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="AC31" s="26">
         <f t="shared" si="9"/>
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="AD31" s="26">
         <f t="shared" si="9"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="AE31" s="26">
         <f t="shared" si="9"/>
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="AF31" s="26">
         <f t="shared" si="9"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="AG31" s="26">
         <f t="shared" si="9"/>
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="AH31" s="26">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="AI31" s="26">
         <f t="shared" si="9"/>
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="AJ31" s="26">
         <f t="shared" si="9"/>
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="AK31" s="26">
         <f t="shared" si="9"/>
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="AL31" s="26">
         <f t="shared" si="9"/>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="AM31" s="26">
         <f t="shared" si="9"/>
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="AN31" s="26">
         <f t="shared" si="9"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AO31" s="26">
         <f t="shared" si="9"/>
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="AP31" s="26">
         <f t="shared" si="9"/>
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="AQ31" s="26">
         <f t="shared" si="9"/>
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="AR31" s="26">
         <f t="shared" si="9"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="AS31" s="26">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="AT31" s="26">
         <f t="shared" si="9"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AU31" s="26">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="AV31" s="26">
         <f t="shared" si="9"/>
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AW31" s="26">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="AX31" s="26">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="AY31" s="26">
         <f t="shared" si="9"/>
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="AZ31" s="26">
         <f t="shared" si="9"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="BA31" s="26">
         <f t="shared" si="9"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="BB31" s="26">
         <f t="shared" si="9"/>
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="BC31" s="26">
         <f t="shared" si="9"/>
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="BD31" s="26">
         <f t="shared" si="9"/>
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="BE31" s="26">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -4921,211 +4951,211 @@
       </c>
       <c r="F33" s="29">
         <f t="shared" ref="F33:BE33" si="10">IF( $B31="Maximum", F31/F32 , IF( 100%-(F31-F32)/F32 &gt; 0, 100%-(F31-F32)/F32, 0) )</f>
-        <v>0.96</v>
+        <v>0.44</v>
       </c>
       <c r="G33" s="29">
         <f t="shared" si="10"/>
-        <v>0.68</v>
+        <v>0.66</v>
       </c>
       <c r="H33" s="29">
         <f t="shared" si="10"/>
-        <v>0.6</v>
+        <v>0.74</v>
       </c>
       <c r="I33" s="29">
         <f t="shared" si="10"/>
-        <v>0.82</v>
+        <v>0.56</v>
       </c>
       <c r="J33" s="29">
         <f t="shared" si="10"/>
-        <v>0.96</v>
+        <v>0.78</v>
       </c>
       <c r="K33" s="29">
         <f t="shared" si="10"/>
-        <v>0.52</v>
+        <v>0.78</v>
       </c>
       <c r="L33" s="29">
         <f t="shared" si="10"/>
-        <v>0.96</v>
+        <v>0.28</v>
       </c>
       <c r="M33" s="29">
         <f t="shared" si="10"/>
-        <v>0.64</v>
+        <v>0.66</v>
       </c>
       <c r="N33" s="29">
         <f t="shared" si="10"/>
-        <v>0.56</v>
+        <v>0.66</v>
       </c>
       <c r="O33" s="29">
         <f t="shared" si="10"/>
-        <v>0.4</v>
+        <v>0.06</v>
       </c>
       <c r="P33" s="29">
         <f t="shared" si="10"/>
-        <v>0.78</v>
+        <v>0.26</v>
       </c>
       <c r="Q33" s="29">
         <f t="shared" si="10"/>
-        <v>0.76</v>
+        <v>0.42</v>
       </c>
       <c r="R33" s="29">
         <f t="shared" si="10"/>
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="S33" s="29">
         <f t="shared" si="10"/>
-        <v>0.26</v>
+        <v>0.96</v>
       </c>
       <c r="T33" s="29">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="U33" s="29">
         <f t="shared" si="10"/>
-        <v>0.18</v>
+        <v>0.32</v>
       </c>
       <c r="V33" s="29">
         <f t="shared" si="10"/>
-        <v>0.34</v>
+        <v>0.06</v>
       </c>
       <c r="W33" s="29">
         <f t="shared" si="10"/>
-        <v>0.9</v>
+        <v>0.28</v>
       </c>
       <c r="X33" s="29">
         <f t="shared" si="10"/>
-        <v>0.34</v>
+        <v>0.32</v>
       </c>
       <c r="Y33" s="29">
         <f t="shared" si="10"/>
-        <v>0.66</v>
+        <v>0.24</v>
       </c>
       <c r="Z33" s="29">
         <f t="shared" si="10"/>
-        <v>0.32</v>
+        <v>0.24</v>
       </c>
       <c r="AA33" s="29">
         <f t="shared" si="10"/>
-        <v>0.8</v>
+        <v>0.68</v>
       </c>
       <c r="AB33" s="29">
         <f t="shared" si="10"/>
-        <v>0.06</v>
+        <v>0.74</v>
       </c>
       <c r="AC33" s="29">
         <f t="shared" si="10"/>
-        <v>0.88</v>
+        <v>0.06</v>
       </c>
       <c r="AD33" s="29">
         <f t="shared" si="10"/>
-        <v>0.52</v>
+        <v>0.36</v>
       </c>
       <c r="AE33" s="29">
         <f t="shared" si="10"/>
-        <v>0.62</v>
+        <v>0.28</v>
       </c>
       <c r="AF33" s="29">
         <f t="shared" si="10"/>
-        <v>0.38</v>
+        <v>0.12</v>
       </c>
       <c r="AG33" s="29">
         <f t="shared" si="10"/>
-        <v>0.68</v>
+        <v>0.02</v>
       </c>
       <c r="AH33" s="29">
         <f t="shared" si="10"/>
-        <v>0.28</v>
+        <v>0.16</v>
       </c>
       <c r="AI33" s="29">
         <f t="shared" si="10"/>
-        <v>0.56</v>
+        <v>0.22</v>
       </c>
       <c r="AJ33" s="29">
         <f t="shared" si="10"/>
-        <v>0.6</v>
+        <v>0.34</v>
       </c>
       <c r="AK33" s="29">
         <f t="shared" si="10"/>
-        <v>0.9</v>
+        <v>0.26</v>
       </c>
       <c r="AL33" s="29">
         <f t="shared" si="10"/>
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="AM33" s="29">
         <f t="shared" si="10"/>
-        <v>0.7</v>
+        <v>0.98</v>
       </c>
       <c r="AN33" s="29">
         <f t="shared" si="10"/>
-        <v>0.22</v>
+        <v>0.08</v>
       </c>
       <c r="AO33" s="29">
         <f t="shared" si="10"/>
-        <v>0.46</v>
+        <v>0.14</v>
       </c>
       <c r="AP33" s="29">
         <f t="shared" si="10"/>
-        <v>0.86</v>
+        <v>0.26</v>
       </c>
       <c r="AQ33" s="29">
         <f t="shared" si="10"/>
-        <v>0.46</v>
+        <v>0.84</v>
       </c>
       <c r="AR33" s="29">
         <f t="shared" si="10"/>
-        <v>0.32</v>
+        <v>0.08</v>
       </c>
       <c r="AS33" s="29">
         <f t="shared" si="10"/>
-        <v>0.04</v>
+        <v>0.76</v>
       </c>
       <c r="AT33" s="29">
         <f t="shared" si="10"/>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AU33" s="29">
         <f t="shared" si="10"/>
-        <v>0.08</v>
+        <v>0.96</v>
       </c>
       <c r="AV33" s="29">
         <f t="shared" si="10"/>
-        <v>0.6</v>
+        <v>0.02</v>
       </c>
       <c r="AW33" s="29">
         <f t="shared" si="10"/>
-        <v>0.24</v>
+        <v>0.78</v>
       </c>
       <c r="AX33" s="29">
         <f t="shared" si="10"/>
-        <v>0.28</v>
+        <v>0.52</v>
       </c>
       <c r="AY33" s="29">
         <f t="shared" si="10"/>
-        <v>0.54</v>
+        <v>1</v>
       </c>
       <c r="AZ33" s="29">
         <f t="shared" si="10"/>
-        <v>0.24</v>
+        <v>0.48</v>
       </c>
       <c r="BA33" s="29">
         <f t="shared" si="10"/>
-        <v>0.7</v>
+        <v>0.66</v>
       </c>
       <c r="BB33" s="29">
         <f t="shared" si="10"/>
-        <v>0.6</v>
+        <v>0.88</v>
       </c>
       <c r="BC33" s="29">
         <f t="shared" si="10"/>
-        <v>0.56</v>
+        <v>0.14</v>
       </c>
       <c r="BD33" s="29">
         <f t="shared" si="10"/>
-        <v>0.82</v>
+        <v>0.36</v>
       </c>
       <c r="BE33" s="29">
         <f t="shared" si="10"/>
-        <v>0.06</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -5137,7 +5167,7 @@
       </c>
       <c r="C34" s="25">
         <f t="array" ref="C34">IF( B35="Short-Term", AVERAGE(F36:BE36)*B36, INDEX(F36:BE36, 1, COUNTA(F36:BE36))*B36 )</f>
-        <v>0.02744230769</v>
+        <v>0.02673076923</v>
       </c>
       <c r="D34" s="6" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(B35=""Short-Term"", SPARKLINE(F36:BE36,IF(B34=""Maximum"", {""charttype"",""column"";""color"",""green""}, {""charttype"",""column"";""color"",""purple""})), SPARKLINE(INDEX(F36:BE36, 1, COUNTA(F36:BE36)) ,IF(B34=""Maximum"", {""charttype"",""bar"";""m"&amp;"ax"",100%;""color1"",""green""}, {""charttype"",""bar"";""max"",100%;""color1"",""purple""})) ) "),"")</f>
@@ -5148,211 +5178,211 @@
       </c>
       <c r="F34" s="26">
         <f t="shared" ref="F34:BE34" si="11">RANDBETWEEN(1,50)</f>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G34" s="26">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="H34" s="26">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="I34" s="26">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J34" s="26">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="K34" s="26">
         <f t="shared" si="11"/>
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="L34" s="26">
         <f t="shared" si="11"/>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="M34" s="26">
         <f t="shared" si="11"/>
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="N34" s="26">
         <f t="shared" si="11"/>
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="O34" s="26">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="P34" s="26">
         <f t="shared" si="11"/>
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="Q34" s="26">
         <f t="shared" si="11"/>
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="R34" s="26">
         <f t="shared" si="11"/>
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="S34" s="26">
         <f t="shared" si="11"/>
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="T34" s="26">
         <f t="shared" si="11"/>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="U34" s="26">
         <f t="shared" si="11"/>
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="V34" s="26">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="W34" s="26">
         <f t="shared" si="11"/>
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="X34" s="26">
         <f t="shared" si="11"/>
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="Y34" s="26">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Z34" s="26">
         <f t="shared" si="11"/>
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AA34" s="26">
         <f t="shared" si="11"/>
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="AB34" s="26">
         <f t="shared" si="11"/>
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="AC34" s="26">
         <f t="shared" si="11"/>
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="AD34" s="26">
         <f t="shared" si="11"/>
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="AE34" s="26">
         <f t="shared" si="11"/>
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="AF34" s="26">
         <f t="shared" si="11"/>
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="AG34" s="26">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AH34" s="26">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="AI34" s="26">
         <f t="shared" si="11"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AJ34" s="26">
         <f t="shared" si="11"/>
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="AK34" s="26">
         <f t="shared" si="11"/>
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="AL34" s="26">
         <f t="shared" si="11"/>
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="AM34" s="26">
         <f t="shared" si="11"/>
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="AN34" s="26">
         <f t="shared" si="11"/>
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="AO34" s="26">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="AP34" s="26">
         <f t="shared" si="11"/>
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="AQ34" s="26">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="AR34" s="26">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="AS34" s="26">
         <f t="shared" si="11"/>
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="AT34" s="26">
         <f t="shared" si="11"/>
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="AU34" s="26">
         <f t="shared" si="11"/>
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AV34" s="26">
         <f t="shared" si="11"/>
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="AW34" s="26">
         <f t="shared" si="11"/>
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="AX34" s="26">
         <f t="shared" si="11"/>
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="AY34" s="26">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AZ34" s="26">
         <f t="shared" si="11"/>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="BA34" s="26">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="BB34" s="26">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="BC34" s="26">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="BD34" s="26">
         <f t="shared" si="11"/>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="BE34" s="26">
         <f t="shared" si="11"/>
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -5531,211 +5561,211 @@
       </c>
       <c r="F36" s="29">
         <f t="shared" ref="F36:BE36" si="12">IF( $B34="Maximum", F34/F35 , IF( 100%-(F34-F35)/F35 &gt; 0, 100%-(F34-F35)/F35, 0) )</f>
-        <v>0.48</v>
+        <v>0.4</v>
       </c>
       <c r="G36" s="29">
         <f t="shared" si="12"/>
-        <v>0.1</v>
+        <v>0.31</v>
       </c>
       <c r="H36" s="29">
         <f t="shared" si="12"/>
-        <v>0.3</v>
+        <v>0.19</v>
       </c>
       <c r="I36" s="29">
         <f t="shared" si="12"/>
-        <v>0.3</v>
+        <v>0.23</v>
       </c>
       <c r="J36" s="29">
         <f t="shared" si="12"/>
-        <v>0.04</v>
+        <v>0.4</v>
       </c>
       <c r="K36" s="29">
         <f t="shared" si="12"/>
-        <v>0.27</v>
+        <v>0.04</v>
       </c>
       <c r="L36" s="29">
         <f t="shared" si="12"/>
-        <v>0.33</v>
+        <v>0.41</v>
       </c>
       <c r="M36" s="29">
         <f t="shared" si="12"/>
-        <v>0.36</v>
+        <v>0.44</v>
       </c>
       <c r="N36" s="29">
         <f t="shared" si="12"/>
-        <v>0.35</v>
+        <v>0.11</v>
       </c>
       <c r="O36" s="29">
         <f t="shared" si="12"/>
-        <v>0.13</v>
+        <v>0.37</v>
       </c>
       <c r="P36" s="29">
         <f t="shared" si="12"/>
-        <v>0.43</v>
+        <v>0.16</v>
       </c>
       <c r="Q36" s="29">
         <f t="shared" si="12"/>
-        <v>0.27</v>
+        <v>0.18</v>
       </c>
       <c r="R36" s="29">
         <f t="shared" si="12"/>
-        <v>0.43</v>
+        <v>0.15</v>
       </c>
       <c r="S36" s="29">
         <f t="shared" si="12"/>
-        <v>0.2</v>
+        <v>0.38</v>
       </c>
       <c r="T36" s="29">
         <f t="shared" si="12"/>
-        <v>0.44</v>
+        <v>0.5</v>
       </c>
       <c r="U36" s="29">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="V36" s="29">
         <f t="shared" si="12"/>
-        <v>0.11</v>
+        <v>0.49</v>
       </c>
       <c r="W36" s="29">
         <f t="shared" si="12"/>
-        <v>0.42</v>
+        <v>0.31</v>
       </c>
       <c r="X36" s="29">
         <f t="shared" si="12"/>
-        <v>0.18</v>
+        <v>0.4</v>
       </c>
       <c r="Y36" s="29">
         <f t="shared" si="12"/>
-        <v>0.15</v>
+        <v>0.28</v>
       </c>
       <c r="Z36" s="29">
         <f t="shared" si="12"/>
-        <v>0.46</v>
+        <v>0.39</v>
       </c>
       <c r="AA36" s="29">
         <f t="shared" si="12"/>
-        <v>0.17</v>
+        <v>0.45</v>
       </c>
       <c r="AB36" s="29">
         <f t="shared" si="12"/>
-        <v>0.35</v>
+        <v>0.29</v>
       </c>
       <c r="AC36" s="29">
         <f t="shared" si="12"/>
-        <v>0.47</v>
+        <v>0.18</v>
       </c>
       <c r="AD36" s="29">
         <f t="shared" si="12"/>
-        <v>0.29</v>
+        <v>0.44</v>
       </c>
       <c r="AE36" s="29">
         <f t="shared" si="12"/>
-        <v>0.39</v>
+        <v>0.32</v>
       </c>
       <c r="AF36" s="29">
         <f t="shared" si="12"/>
-        <v>0.42</v>
+        <v>0.07</v>
       </c>
       <c r="AG36" s="29">
         <f t="shared" si="12"/>
-        <v>0.11</v>
+        <v>0.07</v>
       </c>
       <c r="AH36" s="29">
         <f t="shared" si="12"/>
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
       <c r="AI36" s="29">
         <f t="shared" si="12"/>
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
       <c r="AJ36" s="29">
         <f t="shared" si="12"/>
-        <v>0.27</v>
+        <v>0.15</v>
       </c>
       <c r="AK36" s="29">
         <f t="shared" si="12"/>
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
       <c r="AL36" s="29">
         <f t="shared" si="12"/>
-        <v>0.31</v>
+        <v>0.5</v>
       </c>
       <c r="AM36" s="29">
         <f t="shared" si="12"/>
-        <v>0.37</v>
+        <v>0.15</v>
       </c>
       <c r="AN36" s="29">
         <f t="shared" si="12"/>
-        <v>0.2</v>
+        <v>0.09</v>
       </c>
       <c r="AO36" s="29">
         <f t="shared" si="12"/>
-        <v>0.05</v>
+        <v>0.36</v>
       </c>
       <c r="AP36" s="29">
         <f t="shared" si="12"/>
-        <v>0.22</v>
+        <v>0.5</v>
       </c>
       <c r="AQ36" s="29">
         <f t="shared" si="12"/>
-        <v>0.03</v>
+        <v>0.15</v>
       </c>
       <c r="AR36" s="29">
         <f t="shared" si="12"/>
-        <v>0.04</v>
+        <v>0.35</v>
       </c>
       <c r="AS36" s="29">
         <f t="shared" si="12"/>
-        <v>0.48</v>
+        <v>0.04</v>
       </c>
       <c r="AT36" s="29">
         <f t="shared" si="12"/>
-        <v>0.45</v>
+        <v>0.29</v>
       </c>
       <c r="AU36" s="29">
         <f t="shared" si="12"/>
-        <v>0.33</v>
+        <v>0.08</v>
       </c>
       <c r="AV36" s="29">
         <f t="shared" si="12"/>
-        <v>0.31</v>
+        <v>0.47</v>
       </c>
       <c r="AW36" s="29">
         <f t="shared" si="12"/>
-        <v>0.43</v>
+        <v>0.03</v>
       </c>
       <c r="AX36" s="29">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.21</v>
       </c>
       <c r="AY36" s="29">
         <f t="shared" si="12"/>
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AZ36" s="29">
         <f t="shared" si="12"/>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="BA36" s="29">
         <f t="shared" si="12"/>
-        <v>0.05</v>
+        <v>0.33</v>
       </c>
       <c r="BB36" s="29">
         <f t="shared" si="12"/>
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="BC36" s="29">
         <f t="shared" si="12"/>
-        <v>0.03</v>
+        <v>0.3</v>
       </c>
       <c r="BD36" s="29">
         <f t="shared" si="12"/>
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="BE36" s="29">
         <f t="shared" si="12"/>
-        <v>0.21</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -11278,12 +11308,35 @@
       <formula>LEN(TRIM(F10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B10 B13 B19 B25 B31 B34 B37">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>"Minimum"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10 B13 B19 B25 B31 B34 B37">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"Maximum"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11 B14 B17 B20 B32 B35 B38">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Short-Term"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11 B14 B17 B20 B32 B35 B38">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"Long-Term"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B10 B13 B16 B19 B25 B31 B34 B37">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B10 B13 B19 B25 B31 B34 B37">
       <formula1>"Maximum,Minimum"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B11 B14 B17 B20 B26 B32 B35 B38">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B11 B14 B17 B20 B26 B32 B35 B38">
       <formula1>"Long-Term,Short-Term"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B16">
+      <formula1>"Maximum,Minimum"</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>
@@ -18682,26 +18735,46 @@
     <mergeCell ref="AB6:AE6"/>
     <mergeCell ref="AF6:AI6"/>
   </mergeCells>
+  <conditionalFormatting sqref="B11 B14 B19">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"Short-Term"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11 B14 B19">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"Long-Term"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10 B13 B18">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Minimum"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10 B13 B18">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"Maximum"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F10:BE10 F13:BE13 F18:BE18">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>AND($B10="Maximum",F10&gt;=F11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:BE10 F13:BE13 F18:BE18">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="1" priority="6">
       <formula>AND($B10="Minimum",50%&gt;F12)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:BE10 F13:BE13 F18:BE18">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="7">
       <formula>LEN(TRIM(F10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B10 B13 B18">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B10 B13 B18">
       <formula1>"Maximum,Minimum"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B11 B14 B19">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B11 B14 B19">
       <formula1>"Long-Term,Short-Term"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>